<commit_message>
Actualización de datos 18/07/2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282B8AE7-0532-4FF3-BB16-83FE36AB009A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F371F6C3-FE87-4706-9D22-51FAE81B3D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="600" windowWidth="12405" windowHeight="7935" firstSheet="1" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="1395" yWindow="600" windowWidth="12405" windowHeight="7935" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <sheet name="sc" sheetId="7" r:id="rId8"/>
     <sheet name="tj" sheetId="8" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">tj!$A$1:$E$133</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1107" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -512,9 +515,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2477,7 +2482,7 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="7">
+      <c r="A116" s="4">
         <v>44014</v>
       </c>
       <c r="B116" s="8" t="s">
@@ -2494,7 +2499,7 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="7">
+      <c r="A117" s="4">
         <v>44015</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -2528,7 +2533,7 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="14">
+      <c r="A119" s="4">
         <v>44017</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -2541,6 +2546,227 @@
         <v>2</v>
       </c>
       <c r="E119" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" s="10">
+        <v>57</v>
+      </c>
+      <c r="D120">
+        <v>3</v>
+      </c>
+      <c r="E120" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="11">
+        <v>103</v>
+      </c>
+      <c r="D121">
+        <v>4</v>
+      </c>
+      <c r="E121" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122">
+        <v>176</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123">
+        <v>84</v>
+      </c>
+      <c r="D123">
+        <v>6</v>
+      </c>
+      <c r="E123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="4">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124">
+        <v>99</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125">
+        <v>17</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+      <c r="E125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126">
+        <v>26</v>
+      </c>
+      <c r="D126">
+        <v>3</v>
+      </c>
+      <c r="E126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>24</v>
+      </c>
+      <c r="D127">
+        <v>7</v>
+      </c>
+      <c r="E127">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="4">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128">
+        <v>43</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>53</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130">
+        <v>69</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131">
+        <v>14</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+      <c r="E131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>28</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+      <c r="E132">
         <v>0</v>
       </c>
     </row>
@@ -2551,9 +2777,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4578,6 +4806,227 @@
       </c>
       <c r="E119" s="13">
         <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C120" s="10">
+        <v>33</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121" s="11">
+        <v>68</v>
+      </c>
+      <c r="D121">
+        <v>4</v>
+      </c>
+      <c r="E121" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C122">
+        <v>31</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123">
+        <v>63</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>4</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>133</v>
+      </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
+      <c r="E125">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C126">
+        <v>34</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C128">
+        <v>42</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129">
+        <v>48</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C130">
+        <v>68</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131">
+        <v>46</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+      <c r="E131">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C132">
+        <v>52</v>
+      </c>
+      <c r="D132">
+        <v>5</v>
+      </c>
+      <c r="E132">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -4587,9 +5036,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6614,6 +7065,227 @@
       </c>
       <c r="E119" s="12">
         <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C120" s="10">
+        <v>230</v>
+      </c>
+      <c r="D120">
+        <v>10</v>
+      </c>
+      <c r="E120" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C121" s="11">
+        <v>63</v>
+      </c>
+      <c r="D121">
+        <v>12</v>
+      </c>
+      <c r="E121" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C122">
+        <v>143</v>
+      </c>
+      <c r="D122">
+        <v>8</v>
+      </c>
+      <c r="E122">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123">
+        <v>134</v>
+      </c>
+      <c r="D123">
+        <v>15</v>
+      </c>
+      <c r="E123" s="10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124">
+        <v>146</v>
+      </c>
+      <c r="D124">
+        <v>19</v>
+      </c>
+      <c r="E124" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125">
+        <v>99</v>
+      </c>
+      <c r="D125">
+        <v>19</v>
+      </c>
+      <c r="E125" s="10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C126">
+        <v>174</v>
+      </c>
+      <c r="D126">
+        <v>20</v>
+      </c>
+      <c r="E126" s="10">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C127">
+        <v>127</v>
+      </c>
+      <c r="D127">
+        <v>13</v>
+      </c>
+      <c r="E127" s="10">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <v>153</v>
+      </c>
+      <c r="D128">
+        <v>14</v>
+      </c>
+      <c r="E128" s="10">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C129">
+        <v>276</v>
+      </c>
+      <c r="D129">
+        <v>10</v>
+      </c>
+      <c r="E129" s="10">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C130">
+        <v>182</v>
+      </c>
+      <c r="D130">
+        <v>15</v>
+      </c>
+      <c r="E130" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C131">
+        <v>119</v>
+      </c>
+      <c r="D131">
+        <v>16</v>
+      </c>
+      <c r="E131" s="10">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C132">
+        <v>232</v>
+      </c>
+      <c r="D132">
+        <v>15</v>
+      </c>
+      <c r="E132" s="10">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -6623,9 +7295,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -8650,6 +9324,227 @@
       </c>
       <c r="E119" s="13">
         <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C120" s="10">
+        <v>480</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="11">
+        <v>191</v>
+      </c>
+      <c r="D121">
+        <v>2</v>
+      </c>
+      <c r="E121" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122">
+        <v>275</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C123">
+        <v>225</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+      <c r="E123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C124">
+        <v>328</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125">
+        <v>662</v>
+      </c>
+      <c r="D125">
+        <v>11</v>
+      </c>
+      <c r="E125">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <v>337</v>
+      </c>
+      <c r="D126">
+        <v>4</v>
+      </c>
+      <c r="E126">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127">
+        <v>421</v>
+      </c>
+      <c r="D127">
+        <v>2</v>
+      </c>
+      <c r="E127">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C128">
+        <v>278</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C129">
+        <v>260</v>
+      </c>
+      <c r="D129">
+        <v>5</v>
+      </c>
+      <c r="E129">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C130">
+        <v>314</v>
+      </c>
+      <c r="D130">
+        <v>6</v>
+      </c>
+      <c r="E130">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C131">
+        <v>233</v>
+      </c>
+      <c r="D131">
+        <v>10</v>
+      </c>
+      <c r="E131">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C132">
+        <v>713</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+      <c r="E132">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -8659,9 +9554,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10686,6 +11583,227 @@
       </c>
       <c r="E119" s="13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" s="10">
+        <v>50</v>
+      </c>
+      <c r="D120">
+        <v>7</v>
+      </c>
+      <c r="E120" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" s="11">
+        <v>97</v>
+      </c>
+      <c r="D121">
+        <v>8</v>
+      </c>
+      <c r="E121" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <v>111</v>
+      </c>
+      <c r="D122">
+        <v>8</v>
+      </c>
+      <c r="E122">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123">
+        <v>55</v>
+      </c>
+      <c r="D123">
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C124">
+        <v>89</v>
+      </c>
+      <c r="D124">
+        <v>5</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125">
+        <v>66</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126">
+        <v>85</v>
+      </c>
+      <c r="D126">
+        <v>10</v>
+      </c>
+      <c r="E126">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127">
+        <v>75</v>
+      </c>
+      <c r="D127">
+        <v>4</v>
+      </c>
+      <c r="E127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C128">
+        <v>60</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C129">
+        <v>53</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C130">
+        <v>42</v>
+      </c>
+      <c r="D130">
+        <v>7</v>
+      </c>
+      <c r="E130">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C131">
+        <v>96</v>
+      </c>
+      <c r="D131">
+        <v>9</v>
+      </c>
+      <c r="E131">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132">
+        <v>65</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+      <c r="E132">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -10695,9 +11813,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -12722,6 +13842,227 @@
       </c>
       <c r="E119" s="13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C120" s="10">
+        <v>72</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="E120" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" s="11">
+        <v>20</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126">
+        <v>19</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C127">
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>8</v>
+      </c>
+      <c r="E127">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>4</v>
+      </c>
+      <c r="E128">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>9</v>
+      </c>
+      <c r="E129">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>5</v>
+      </c>
+      <c r="E130">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>12</v>
+      </c>
+      <c r="D131">
+        <v>4</v>
+      </c>
+      <c r="E131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <v>121</v>
+      </c>
+      <c r="D132">
+        <v>7</v>
+      </c>
+      <c r="E132">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -12731,9 +14072,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -14758,6 +16101,227 @@
       </c>
       <c r="E119" s="13">
         <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" s="10">
+        <v>21</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" s="11">
+        <v>19</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122">
+        <v>30</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123">
+        <v>13</v>
+      </c>
+      <c r="D123">
+        <v>4</v>
+      </c>
+      <c r="E123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125">
+        <v>11</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126">
+        <v>37</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C127">
+        <v>24</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C128">
+        <v>50</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C129">
+        <v>31</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130">
+        <v>60</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C131">
+        <v>26</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132">
+        <v>11</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -14767,9 +16331,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -16794,6 +18360,227 @@
       </c>
       <c r="E119" s="13">
         <v>344</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C120" s="10">
+        <v>201</v>
+      </c>
+      <c r="D120">
+        <v>18</v>
+      </c>
+      <c r="E120" s="12">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C121" s="11">
+        <v>445</v>
+      </c>
+      <c r="D121">
+        <v>23</v>
+      </c>
+      <c r="E121" s="13">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C122">
+        <v>528</v>
+      </c>
+      <c r="D122">
+        <v>24</v>
+      </c>
+      <c r="E122">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C123">
+        <v>485</v>
+      </c>
+      <c r="D123">
+        <v>23</v>
+      </c>
+      <c r="E123">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C124">
+        <v>614</v>
+      </c>
+      <c r="D124">
+        <v>26</v>
+      </c>
+      <c r="E124">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C125">
+        <v>600</v>
+      </c>
+      <c r="D125">
+        <v>13</v>
+      </c>
+      <c r="E125">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126">
+        <v>275</v>
+      </c>
+      <c r="D126">
+        <v>9</v>
+      </c>
+      <c r="E126">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C127">
+        <v>360</v>
+      </c>
+      <c r="D127">
+        <v>24</v>
+      </c>
+      <c r="E127">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C128">
+        <v>864</v>
+      </c>
+      <c r="D128">
+        <v>7</v>
+      </c>
+      <c r="E128">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C129">
+        <v>547</v>
+      </c>
+      <c r="D129">
+        <v>16</v>
+      </c>
+      <c r="E129">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C130">
+        <v>1073</v>
+      </c>
+      <c r="D130">
+        <v>5</v>
+      </c>
+      <c r="E130">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C131">
+        <v>1245</v>
+      </c>
+      <c r="D131">
+        <v>17</v>
+      </c>
+      <c r="E131">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C132">
+        <v>495</v>
+      </c>
+      <c r="D132">
+        <v>19</v>
+      </c>
+      <c r="E132">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -16803,9 +18590,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E119"/>
+  <dimension ref="A1:E132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A110" workbookViewId="0">
+      <selection activeCell="E133" sqref="C133:E133"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -18835,6 +20624,227 @@
         <v>0</v>
       </c>
     </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="14">
+        <v>44018</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C120" s="10">
+        <v>68</v>
+      </c>
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="E120" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="14">
+        <v>44019</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="11">
+        <v>30</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="14">
+        <v>44020</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122">
+        <v>145</v>
+      </c>
+      <c r="D122">
+        <v>3</v>
+      </c>
+      <c r="E122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="14">
+        <v>44021</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C123">
+        <v>70</v>
+      </c>
+      <c r="D123">
+        <v>5</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="14">
+        <v>44022</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C124">
+        <v>170</v>
+      </c>
+      <c r="D124">
+        <v>2</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="14">
+        <v>44023</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C125">
+        <v>47</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
+      </c>
+      <c r="E125">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="14">
+        <v>44024</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="14">
+        <v>44025</v>
+      </c>
+      <c r="B127" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127">
+        <v>32</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="14">
+        <v>44026</v>
+      </c>
+      <c r="B128" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128">
+        <v>127</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="14">
+        <v>44027</v>
+      </c>
+      <c r="B129" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C129">
+        <v>83</v>
+      </c>
+      <c r="D129">
+        <v>3</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="14">
+        <v>44028</v>
+      </c>
+      <c r="B130" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130">
+        <v>130</v>
+      </c>
+      <c r="D130">
+        <v>2</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="14">
+        <v>44029</v>
+      </c>
+      <c r="B131" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C131">
+        <v>155</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+      <c r="E131">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="14">
+        <v>44030</v>
+      </c>
+      <c r="B132" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C132">
+        <v>319</v>
+      </c>
+      <c r="D132">
+        <v>6</v>
+      </c>
+      <c r="E132">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado a 19 julio 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F371F6C3-FE87-4706-9D22-51FAE81B3D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEEDE3A-D4CA-4FD4-A5CB-8CFBA0C845EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="600" windowWidth="12405" windowHeight="7935" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="26160" windowHeight="11760" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
-    <sheet name="ch" sheetId="3" r:id="rId2"/>
-    <sheet name="cb" sheetId="9" r:id="rId3"/>
+    <sheet name="cb" sheetId="9" r:id="rId2"/>
+    <sheet name="ch" sheetId="3" r:id="rId3"/>
     <sheet name="lp" sheetId="4" r:id="rId4"/>
     <sheet name="or" sheetId="5" r:id="rId5"/>
     <sheet name="pn" sheetId="2" r:id="rId6"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,17 +2770,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133">
+        <v>24</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+    <sheetView topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2807,7 +2824,7 @@
         <v>43900</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -2824,7 +2841,7 @@
         <v>43901</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
@@ -2841,7 +2858,7 @@
         <v>43902</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -2858,10 +2875,10 @@
         <v>43903</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -2875,7 +2892,7 @@
         <v>43904</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -2892,7 +2909,7 @@
         <v>43905</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2909,7 +2926,7 @@
         <v>43906</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -2926,7 +2943,7 @@
         <v>43907</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -2943,7 +2960,7 @@
         <v>43908</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="5">
         <v>0</v>
@@ -2960,10 +2977,10 @@
         <v>43909</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="8">
         <v>0</v>
@@ -2977,7 +2994,7 @@
         <v>43910</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
@@ -2994,7 +3011,7 @@
         <v>43911</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -3011,10 +3028,10 @@
         <v>43912</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
@@ -3028,7 +3045,7 @@
         <v>43913</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -3045,7 +3062,7 @@
         <v>43914</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -3062,7 +3079,7 @@
         <v>43915</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3079,10 +3096,10 @@
         <v>43916</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D18" s="5">
         <v>0</v>
@@ -3096,10 +3113,10 @@
         <v>43917</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19" s="8">
         <v>0</v>
@@ -3113,7 +3130,7 @@
         <v>43918</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -3130,10 +3147,10 @@
         <v>43919</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D21" s="8">
         <v>0</v>
@@ -3147,10 +3164,10 @@
         <v>43920</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
@@ -3164,7 +3181,7 @@
         <v>43921</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="8">
         <v>0</v>
@@ -3181,10 +3198,10 @@
         <v>43922</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5">
         <v>0</v>
@@ -3198,10 +3215,10 @@
         <v>43923</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="8">
         <v>0</v>
@@ -3215,10 +3232,10 @@
         <v>43924</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="5">
         <v>0</v>
@@ -3232,10 +3249,10 @@
         <v>43925</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="8">
         <v>0</v>
@@ -3249,13 +3266,13 @@
         <v>43926</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
@@ -3266,13 +3283,13 @@
         <v>43927</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
       </c>
       <c r="D29" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="9">
         <v>0</v>
@@ -3283,10 +3300,10 @@
         <v>43928</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D30" s="5">
         <v>0</v>
@@ -3300,10 +3317,10 @@
         <v>43929</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D31" s="8">
         <v>0</v>
@@ -3317,10 +3334,10 @@
         <v>43930</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -3334,7 +3351,7 @@
         <v>43931</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="8">
         <v>0</v>
@@ -3351,13 +3368,13 @@
         <v>43932</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
@@ -3368,10 +3385,10 @@
         <v>43933</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D35" s="8">
         <v>0</v>
@@ -3385,10 +3402,10 @@
         <v>43934</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D36" s="5">
         <v>0</v>
@@ -3402,10 +3419,10 @@
         <v>43935</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D37" s="8">
         <v>0</v>
@@ -3419,10 +3436,10 @@
         <v>43936</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D38" s="5">
         <v>0</v>
@@ -3436,7 +3453,7 @@
         <v>43937</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -3445,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3453,10 +3470,10 @@
         <v>43938</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="5">
         <v>0</v>
@@ -3470,7 +3487,7 @@
         <v>43939</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="8">
         <v>0</v>
@@ -3487,13 +3504,13 @@
         <v>43940</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="6">
         <v>0</v>
@@ -3504,16 +3521,16 @@
         <v>43941</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="8">
         <v>0</v>
       </c>
       <c r="D43" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3521,10 +3538,10 @@
         <v>43942</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C44" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="5">
         <v>0</v>
@@ -3538,10 +3555,10 @@
         <v>43943</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="8">
         <v>0</v>
@@ -3555,10 +3572,10 @@
         <v>43944</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C46" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D46" s="5">
         <v>0</v>
@@ -3572,10 +3589,10 @@
         <v>43945</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D47" s="8">
         <v>0</v>
@@ -3589,10 +3606,10 @@
         <v>43946</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="5">
         <v>0</v>
@@ -3606,10 +3623,10 @@
         <v>43947</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D49" s="8">
         <v>0</v>
@@ -3623,16 +3640,16 @@
         <v>43948</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D50" s="5">
         <v>0</v>
       </c>
       <c r="E50" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3640,10 +3657,10 @@
         <v>43949</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="8">
         <v>0</v>
@@ -3657,10 +3674,10 @@
         <v>43950</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C52" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="5">
         <v>0</v>
@@ -3674,7 +3691,7 @@
         <v>43951</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" s="8">
         <v>0</v>
@@ -3683,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3691,10 +3708,10 @@
         <v>43952</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C54" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="5">
         <v>0</v>
@@ -3708,10 +3725,10 @@
         <v>43953</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="8">
         <v>0</v>
@@ -3725,7 +3742,7 @@
         <v>43954</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="5">
         <v>0</v>
@@ -3742,13 +3759,13 @@
         <v>43955</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" s="8">
         <v>1</v>
       </c>
       <c r="D57" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="9">
         <v>0</v>
@@ -3759,16 +3776,16 @@
         <v>43956</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" s="5">
         <v>0</v>
       </c>
       <c r="E58" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3776,7 +3793,7 @@
         <v>43957</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" s="8">
         <v>0</v>
@@ -3793,10 +3810,10 @@
         <v>43958</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D60" s="5">
         <v>0</v>
@@ -3810,16 +3827,16 @@
         <v>43959</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61" s="8">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D61" s="8">
         <v>0</v>
       </c>
       <c r="E61" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3827,10 +3844,10 @@
         <v>43960</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D62" s="5">
         <v>0</v>
@@ -3844,10 +3861,10 @@
         <v>43961</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C63" s="8">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D63" s="8">
         <v>0</v>
@@ -3861,16 +3878,16 @@
         <v>43962</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,13 +3895,13 @@
         <v>43963</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" s="8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D65" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65" s="9">
         <v>0</v>
@@ -3895,13 +3912,13 @@
         <v>43964</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C66" s="5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D66" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66" s="6">
         <v>0</v>
@@ -3912,10 +3929,10 @@
         <v>43965</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67" s="8">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D67" s="8">
         <v>0</v>
@@ -3929,13 +3946,13 @@
         <v>43966</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="5">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D68" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68" s="6">
         <v>0</v>
@@ -3946,16 +3963,16 @@
         <v>43967</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C69" s="8">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D69" s="8">
         <v>0</v>
       </c>
       <c r="E69" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3963,10 +3980,10 @@
         <v>43968</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D70" s="5">
         <v>0</v>
@@ -3980,13 +3997,13 @@
         <v>43969</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" s="8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D71" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="9">
         <v>0</v>
@@ -3997,16 +4014,16 @@
         <v>43970</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" s="5">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D72" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72" s="6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -4014,16 +4031,16 @@
         <v>43971</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" s="8">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D73" s="8">
         <v>0</v>
       </c>
       <c r="E73" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -4031,10 +4048,10 @@
         <v>43972</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D74" s="5">
         <v>0</v>
@@ -4048,16 +4065,16 @@
         <v>43973</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" s="8">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D75" s="8">
         <v>0</v>
       </c>
       <c r="E75" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -4065,13 +4082,13 @@
         <v>43974</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" s="5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D76" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E76" s="6">
         <v>0</v>
@@ -4082,10 +4099,10 @@
         <v>43975</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" s="8">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="D77" s="8">
         <v>0</v>
@@ -4099,13 +4116,13 @@
         <v>43976</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D78" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E78" s="6">
         <v>0</v>
@@ -4116,16 +4133,16 @@
         <v>43977</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D79" s="8">
         <v>0</v>
       </c>
       <c r="E79" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -4133,10 +4150,10 @@
         <v>43978</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" s="5">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D80" s="5">
         <v>0</v>
@@ -4150,13 +4167,13 @@
         <v>43979</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" s="8">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D81" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81" s="9">
         <v>0</v>
@@ -4167,13 +4184,13 @@
         <v>43980</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" s="5">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D82" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E82" s="6">
         <v>0</v>
@@ -4184,16 +4201,16 @@
         <v>43981</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C83" s="8">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D83" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E83" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4201,16 +4218,16 @@
         <v>43982</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C84" s="5">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="D84" s="5">
         <v>0</v>
       </c>
       <c r="E84" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4218,13 +4235,13 @@
         <v>43983</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" s="8">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="D85" s="8">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E85" s="9">
         <v>0</v>
@@ -4235,16 +4252,16 @@
         <v>43984</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C86" s="5">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="D86" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E86" s="6">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4252,13 +4269,13 @@
         <v>43985</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" s="8">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="D87" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E87" s="9">
         <v>0</v>
@@ -4269,16 +4286,16 @@
         <v>43986</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C88" s="5">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="D88" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E88" s="6">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4286,13 +4303,13 @@
         <v>43987</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C89" s="8">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D89" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E89" s="9">
         <v>0</v>
@@ -4303,13 +4320,13 @@
         <v>43988</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C90" s="5">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D90" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90" s="6">
         <v>0</v>
@@ -4320,10 +4337,10 @@
         <v>43989</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C91" s="8">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D91" s="8">
         <v>0</v>
@@ -4337,13 +4354,13 @@
         <v>43990</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="5">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="D92" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E92" s="6">
         <v>0</v>
@@ -4354,13 +4371,13 @@
         <v>43991</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" s="8">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D93" s="8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E93" s="9">
         <v>0</v>
@@ -4371,13 +4388,13 @@
         <v>43992</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C94" s="5">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="D94" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94" s="6">
         <v>0</v>
@@ -4388,16 +4405,16 @@
         <v>43993</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95" s="8">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="D95" s="8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E95" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4405,13 +4422,13 @@
         <v>43994</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C96" s="5">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="D96" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E96" s="6">
         <v>0</v>
@@ -4422,13 +4439,13 @@
         <v>43995</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C97" s="8">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="D97" s="8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E97" s="9">
         <v>0</v>
@@ -4439,13 +4456,13 @@
         <v>43996</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C98" s="5">
-        <v>2</v>
+        <v>186</v>
       </c>
       <c r="D98" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E98" s="6">
         <v>0</v>
@@ -4456,16 +4473,16 @@
         <v>43997</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99" s="8">
-        <v>15</v>
+        <v>155</v>
       </c>
       <c r="D99" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E99" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4473,13 +4490,13 @@
         <v>43998</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C100" s="5">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="D100" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E100" s="6">
         <v>0</v>
@@ -4490,16 +4507,16 @@
         <v>43999</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" s="8">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="D101" s="8">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E101" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4507,16 +4524,16 @@
         <v>44000</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C102" s="5">
-        <v>51</v>
+        <v>138</v>
       </c>
       <c r="D102" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E102" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4524,16 +4541,16 @@
         <v>44001</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" s="8">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="D103" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E103" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4541,13 +4558,13 @@
         <v>44002</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C104" s="5">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D104" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E104" s="6">
         <v>0</v>
@@ -4558,16 +4575,16 @@
         <v>44003</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C105" s="8">
-        <v>48</v>
+        <v>191</v>
       </c>
       <c r="D105" s="8">
         <v>6</v>
       </c>
       <c r="E105" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4575,16 +4592,16 @@
         <v>44004</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C106" s="5">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="D106" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E106" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4592,16 +4609,16 @@
         <v>44005</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107" s="8">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="D107" s="8">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E107" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4609,16 +4626,16 @@
         <v>44006</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C108" s="5">
-        <v>40</v>
+        <v>145</v>
       </c>
       <c r="D108" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E108" s="6">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4626,16 +4643,16 @@
         <v>44007</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C109" s="8">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D109" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E109" s="9">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4643,16 +4660,16 @@
         <v>44008</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C110" s="5">
-        <v>54</v>
+        <v>263</v>
       </c>
       <c r="D110" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E110" s="6">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4660,16 +4677,16 @@
         <v>44009</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C111" s="8">
-        <v>54</v>
+        <v>183</v>
       </c>
       <c r="D111" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E111" s="9">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4677,13 +4694,13 @@
         <v>44010</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C112" s="10">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D112" s="10">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E112" s="12">
         <v>0</v>
@@ -4694,16 +4711,16 @@
         <v>44011</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C113" s="11">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E113" s="13">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4711,13 +4728,13 @@
         <v>44012</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C114" s="10">
-        <v>63</v>
+        <v>139</v>
       </c>
       <c r="D114">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E114" s="12">
         <v>0</v>
@@ -4728,16 +4745,16 @@
         <v>44013</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115" s="11">
-        <v>59</v>
+        <v>104</v>
       </c>
       <c r="D115">
-        <v>2</v>
-      </c>
-      <c r="E115" s="13">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="E115" s="12">
+        <v>15</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4745,16 +4762,16 @@
         <v>44014</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C116" s="10">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="D116">
-        <v>1</v>
-      </c>
-      <c r="E116" s="12">
-        <v>5</v>
+        <v>12</v>
+      </c>
+      <c r="E116" s="13">
+        <v>17</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4762,16 +4779,16 @@
         <v>44015</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C117" s="11">
-        <v>41</v>
+        <v>253</v>
       </c>
       <c r="D117">
-        <v>5</v>
-      </c>
-      <c r="E117" s="13">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="E117" s="12">
+        <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4779,254 +4796,271 @@
         <v>44016</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C118" s="10">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E118" s="12">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
         <v>44017</v>
       </c>
-      <c r="B119" s="14" t="s">
-        <v>3</v>
+      <c r="B119" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C119" s="11">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D119">
-        <v>1</v>
-      </c>
-      <c r="E119" s="13">
-        <v>4</v>
+        <v>20</v>
+      </c>
+      <c r="E119" s="12">
+        <v>36</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <v>44018</v>
       </c>
-      <c r="B120" s="14" t="s">
-        <v>3</v>
+      <c r="B120" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C120" s="10">
-        <v>33</v>
+        <v>230</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E120" s="12">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="14">
         <v>44019</v>
       </c>
-      <c r="B121" s="14" t="s">
-        <v>3</v>
+      <c r="B121" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C121" s="11">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D121">
-        <v>4</v>
-      </c>
-      <c r="E121" s="13">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E121" s="12">
+        <v>28</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
         <v>44020</v>
       </c>
-      <c r="B122" s="14" t="s">
-        <v>3</v>
+      <c r="B122" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C122">
-        <v>31</v>
+        <v>143</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E122">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="14">
         <v>44021</v>
       </c>
-      <c r="B123" s="14" t="s">
-        <v>3</v>
+      <c r="B123" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C123">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="D123">
-        <v>2</v>
-      </c>
-      <c r="E123">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="E123" s="10">
+        <v>29</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="14">
         <v>44022</v>
       </c>
-      <c r="B124" s="14" t="s">
-        <v>3</v>
+      <c r="B124" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C124">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="D124">
-        <v>4</v>
-      </c>
-      <c r="E124">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="E124" s="10">
+        <v>31</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="14">
         <v>44023</v>
       </c>
-      <c r="B125" s="14" t="s">
-        <v>3</v>
+      <c r="B125" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C125">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="D125">
-        <v>2</v>
-      </c>
-      <c r="E125">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="E125" s="10">
+        <v>36</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="14">
         <v>44024</v>
       </c>
-      <c r="B126" s="14" t="s">
-        <v>3</v>
+      <c r="B126" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C126">
-        <v>34</v>
+        <v>174</v>
       </c>
       <c r="D126">
-        <v>2</v>
-      </c>
-      <c r="E126">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="E126" s="10">
+        <v>58</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="14">
         <v>44025</v>
       </c>
-      <c r="B127" s="14" t="s">
-        <v>3</v>
+      <c r="B127" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D127">
-        <v>0</v>
-      </c>
-      <c r="E127">
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="E127" s="10">
+        <v>67</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="14">
         <v>44026</v>
       </c>
-      <c r="B128" s="14" t="s">
-        <v>3</v>
+      <c r="B128" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C128">
-        <v>42</v>
+        <v>153</v>
       </c>
       <c r="D128">
-        <v>0</v>
-      </c>
-      <c r="E128">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="E128" s="10">
+        <v>44</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="14">
         <v>44027</v>
       </c>
-      <c r="B129" s="14" t="s">
-        <v>3</v>
+      <c r="B129" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C129">
-        <v>48</v>
+        <v>276</v>
       </c>
       <c r="D129">
-        <v>0</v>
-      </c>
-      <c r="E129">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E129" s="10">
+        <v>84</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="14">
         <v>44028</v>
       </c>
-      <c r="B130" s="14" t="s">
-        <v>3</v>
+      <c r="B130" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C130">
-        <v>68</v>
+        <v>182</v>
       </c>
       <c r="D130">
-        <v>1</v>
-      </c>
-      <c r="E130">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="E130" s="10">
+        <v>75</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="14">
         <v>44029</v>
       </c>
-      <c r="B131" s="14" t="s">
-        <v>3</v>
+      <c r="B131" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C131">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D131">
-        <v>2</v>
-      </c>
-      <c r="E131">
-        <v>26</v>
+        <v>16</v>
+      </c>
+      <c r="E131" s="10">
+        <v>212</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="14">
         <v>44030</v>
       </c>
-      <c r="B132" s="14" t="s">
-        <v>3</v>
+      <c r="B132" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="C132">
-        <v>52</v>
+        <v>232</v>
       </c>
       <c r="D132">
-        <v>5</v>
-      </c>
-      <c r="E132">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="E132" s="10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <v>129</v>
+      </c>
+      <c r="D133">
+        <v>15</v>
+      </c>
+      <c r="E133" s="10">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -5035,11 +5069,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5066,7 +5100,7 @@
         <v>43900</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="5">
         <v>0</v>
@@ -5083,7 +5117,7 @@
         <v>43901</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
@@ -5100,7 +5134,7 @@
         <v>43902</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5">
         <v>0</v>
@@ -5117,10 +5151,10 @@
         <v>43903</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" s="8">
         <v>0</v>
@@ -5134,7 +5168,7 @@
         <v>43904</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="5">
         <v>0</v>
@@ -5151,7 +5185,7 @@
         <v>43905</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -5168,7 +5202,7 @@
         <v>43906</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" s="5">
         <v>0</v>
@@ -5185,7 +5219,7 @@
         <v>43907</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -5202,7 +5236,7 @@
         <v>43908</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="5">
         <v>0</v>
@@ -5219,10 +5253,10 @@
         <v>43909</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" s="8">
         <v>0</v>
@@ -5236,7 +5270,7 @@
         <v>43910</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12" s="5">
         <v>0</v>
@@ -5253,7 +5287,7 @@
         <v>43911</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -5270,10 +5304,10 @@
         <v>43912</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" s="5">
         <v>0</v>
@@ -5287,7 +5321,7 @@
         <v>43913</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -5304,7 +5338,7 @@
         <v>43914</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" s="5">
         <v>0</v>
@@ -5321,7 +5355,7 @@
         <v>43915</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -5338,10 +5372,10 @@
         <v>43916</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D18" s="5">
         <v>0</v>
@@ -5355,10 +5389,10 @@
         <v>43917</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" s="8">
         <v>0</v>
@@ -5372,7 +5406,7 @@
         <v>43918</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" s="5">
         <v>0</v>
@@ -5389,10 +5423,10 @@
         <v>43919</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" s="8">
         <v>0</v>
@@ -5406,10 +5440,10 @@
         <v>43920</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
@@ -5423,7 +5457,7 @@
         <v>43921</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23" s="8">
         <v>0</v>
@@ -5440,10 +5474,10 @@
         <v>43922</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" s="5">
         <v>0</v>
@@ -5457,10 +5491,10 @@
         <v>43923</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25" s="8">
         <v>0</v>
@@ -5474,10 +5508,10 @@
         <v>43924</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D26" s="5">
         <v>0</v>
@@ -5491,10 +5525,10 @@
         <v>43925</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="8">
         <v>0</v>
@@ -5508,13 +5542,13 @@
         <v>43926</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="5">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D28" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
@@ -5525,13 +5559,13 @@
         <v>43927</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
       </c>
       <c r="D29" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="9">
         <v>0</v>
@@ -5542,10 +5576,10 @@
         <v>43928</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C30" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D30" s="5">
         <v>0</v>
@@ -5559,10 +5593,10 @@
         <v>43929</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D31" s="8">
         <v>0</v>
@@ -5576,10 +5610,10 @@
         <v>43930</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C32" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -5593,7 +5627,7 @@
         <v>43931</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33" s="8">
         <v>0</v>
@@ -5610,13 +5644,13 @@
         <v>43932</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E34" s="6">
         <v>0</v>
@@ -5627,10 +5661,10 @@
         <v>43933</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D35" s="8">
         <v>0</v>
@@ -5644,10 +5678,10 @@
         <v>43934</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D36" s="5">
         <v>0</v>
@@ -5661,10 +5695,10 @@
         <v>43935</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D37" s="8">
         <v>0</v>
@@ -5678,10 +5712,10 @@
         <v>43936</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C38" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D38" s="5">
         <v>0</v>
@@ -5695,7 +5729,7 @@
         <v>43937</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -5704,7 +5738,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -5712,10 +5746,10 @@
         <v>43938</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" s="5">
         <v>0</v>
@@ -5729,7 +5763,7 @@
         <v>43939</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" s="8">
         <v>0</v>
@@ -5746,13 +5780,13 @@
         <v>43940</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="6">
         <v>0</v>
@@ -5763,16 +5797,16 @@
         <v>43941</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" s="8">
         <v>0</v>
       </c>
       <c r="D43" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="9">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -5780,10 +5814,10 @@
         <v>43942</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C44" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="5">
         <v>0</v>
@@ -5797,10 +5831,10 @@
         <v>43943</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C45" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45" s="8">
         <v>0</v>
@@ -5814,10 +5848,10 @@
         <v>43944</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46" s="5">
         <v>0</v>
@@ -5831,10 +5865,10 @@
         <v>43945</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D47" s="8">
         <v>0</v>
@@ -5848,10 +5882,10 @@
         <v>43946</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" s="5">
         <v>0</v>
@@ -5865,10 +5899,10 @@
         <v>43947</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C49" s="8">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D49" s="8">
         <v>0</v>
@@ -5882,16 +5916,16 @@
         <v>43948</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="5">
         <v>0</v>
       </c>
       <c r="E50" s="6">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -5899,10 +5933,10 @@
         <v>43949</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C51" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="8">
         <v>0</v>
@@ -5916,10 +5950,10 @@
         <v>43950</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C52" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="5">
         <v>0</v>
@@ -5933,7 +5967,7 @@
         <v>43951</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C53" s="8">
         <v>0</v>
@@ -5942,7 +5976,7 @@
         <v>0</v>
       </c>
       <c r="E53" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -5950,10 +5984,10 @@
         <v>43952</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C54" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="5">
         <v>0</v>
@@ -5967,10 +6001,10 @@
         <v>43953</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" s="8">
         <v>0</v>
@@ -5984,7 +6018,7 @@
         <v>43954</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C56" s="5">
         <v>0</v>
@@ -6001,13 +6035,13 @@
         <v>43955</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="8">
         <v>1</v>
       </c>
       <c r="D57" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57" s="9">
         <v>0</v>
@@ -6018,16 +6052,16 @@
         <v>43956</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="5">
         <v>0</v>
       </c>
       <c r="E58" s="6">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -6035,7 +6069,7 @@
         <v>43957</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" s="8">
         <v>0</v>
@@ -6052,10 +6086,10 @@
         <v>43958</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D60" s="5">
         <v>0</v>
@@ -6069,16 +6103,16 @@
         <v>43959</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C61" s="8">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D61" s="8">
         <v>0</v>
       </c>
       <c r="E61" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -6086,10 +6120,10 @@
         <v>43960</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C62" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D62" s="5">
         <v>0</v>
@@ -6103,10 +6137,10 @@
         <v>43961</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C63" s="8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D63" s="8">
         <v>0</v>
@@ -6120,16 +6154,16 @@
         <v>43962</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -6137,13 +6171,13 @@
         <v>43963</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C65" s="8">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D65" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" s="9">
         <v>0</v>
@@ -6154,13 +6188,13 @@
         <v>43964</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C66" s="5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D66" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" s="6">
         <v>0</v>
@@ -6171,10 +6205,10 @@
         <v>43965</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C67" s="8">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D67" s="8">
         <v>0</v>
@@ -6188,13 +6222,13 @@
         <v>43966</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C68" s="5">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="6">
         <v>0</v>
@@ -6205,16 +6239,16 @@
         <v>43967</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C69" s="8">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D69" s="8">
         <v>0</v>
       </c>
       <c r="E69" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -6222,10 +6256,10 @@
         <v>43968</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C70" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D70" s="5">
         <v>0</v>
@@ -6239,13 +6273,13 @@
         <v>43969</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71" s="8">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D71" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="9">
         <v>0</v>
@@ -6256,16 +6290,16 @@
         <v>43970</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C72" s="5">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D72" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -6273,16 +6307,16 @@
         <v>43971</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C73" s="8">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D73" s="8">
         <v>0</v>
       </c>
       <c r="E73" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -6290,10 +6324,10 @@
         <v>43972</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D74" s="5">
         <v>0</v>
@@ -6307,16 +6341,16 @@
         <v>43973</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C75" s="8">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D75" s="8">
         <v>0</v>
       </c>
       <c r="E75" s="9">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -6324,13 +6358,13 @@
         <v>43974</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C76" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D76" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E76" s="6">
         <v>0</v>
@@ -6341,10 +6375,10 @@
         <v>43975</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C77" s="8">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D77" s="8">
         <v>0</v>
@@ -6358,13 +6392,13 @@
         <v>43976</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C78" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D78" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E78" s="6">
         <v>0</v>
@@ -6375,16 +6409,16 @@
         <v>43977</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C79" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D79" s="8">
         <v>0</v>
       </c>
       <c r="E79" s="9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -6392,10 +6426,10 @@
         <v>43978</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C80" s="5">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="D80" s="5">
         <v>0</v>
@@ -6409,13 +6443,13 @@
         <v>43979</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C81" s="8">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="D81" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81" s="9">
         <v>0</v>
@@ -6426,13 +6460,13 @@
         <v>43980</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C82" s="5">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D82" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E82" s="6">
         <v>0</v>
@@ -6443,16 +6477,16 @@
         <v>43981</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C83" s="8">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D83" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E83" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -6460,16 +6494,16 @@
         <v>43982</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84" s="5">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="D84" s="5">
         <v>0</v>
       </c>
       <c r="E84" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -6477,13 +6511,13 @@
         <v>43983</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C85" s="8">
-        <v>103</v>
+        <v>2</v>
       </c>
       <c r="D85" s="8">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E85" s="9">
         <v>0</v>
@@ -6494,16 +6528,16 @@
         <v>43984</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C86" s="5">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="D86" s="5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E86" s="6">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -6511,13 +6545,13 @@
         <v>43985</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C87" s="8">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="D87" s="8">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E87" s="9">
         <v>0</v>
@@ -6528,16 +6562,16 @@
         <v>43986</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C88" s="5">
-        <v>47</v>
+        <v>1</v>
       </c>
       <c r="D88" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E88" s="6">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -6545,13 +6579,13 @@
         <v>43987</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C89" s="8">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="D89" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E89" s="9">
         <v>0</v>
@@ -6562,13 +6596,13 @@
         <v>43988</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C90" s="5">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="6">
         <v>0</v>
@@ -6579,10 +6613,10 @@
         <v>43989</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C91" s="8">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D91" s="8">
         <v>0</v>
@@ -6596,13 +6630,13 @@
         <v>43990</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C92" s="5">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="D92" s="5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E92" s="6">
         <v>0</v>
@@ -6613,13 +6647,13 @@
         <v>43991</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C93" s="8">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="D93" s="8">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E93" s="9">
         <v>0</v>
@@ -6630,13 +6664,13 @@
         <v>43992</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C94" s="5">
-        <v>66</v>
+        <v>18</v>
       </c>
       <c r="D94" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94" s="6">
         <v>0</v>
@@ -6647,16 +6681,16 @@
         <v>43993</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C95" s="8">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="D95" s="8">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E95" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -6664,13 +6698,13 @@
         <v>43994</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C96" s="5">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="D96" s="5">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E96" s="6">
         <v>0</v>
@@ -6681,13 +6715,13 @@
         <v>43995</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C97" s="8">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="D97" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E97" s="9">
         <v>0</v>
@@ -6698,13 +6732,13 @@
         <v>43996</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C98" s="5">
-        <v>186</v>
+        <v>2</v>
       </c>
       <c r="D98" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E98" s="6">
         <v>0</v>
@@ -6715,16 +6749,16 @@
         <v>43997</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C99" s="8">
-        <v>155</v>
+        <v>15</v>
       </c>
       <c r="D99" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E99" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -6732,13 +6766,13 @@
         <v>43998</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C100" s="5">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="D100" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E100" s="6">
         <v>0</v>
@@ -6749,16 +6783,16 @@
         <v>43999</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C101" s="8">
-        <v>126</v>
+        <v>5</v>
       </c>
       <c r="D101" s="8">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E101" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -6766,16 +6800,16 @@
         <v>44000</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C102" s="5">
-        <v>138</v>
+        <v>51</v>
       </c>
       <c r="D102" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E102" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -6783,16 +6817,16 @@
         <v>44001</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C103" s="8">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="D103" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E103" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -6800,13 +6834,13 @@
         <v>44002</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C104" s="5">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D104" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E104" s="6">
         <v>0</v>
@@ -6817,16 +6851,16 @@
         <v>44003</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C105" s="8">
-        <v>191</v>
+        <v>48</v>
       </c>
       <c r="D105" s="8">
         <v>6</v>
       </c>
       <c r="E105" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -6834,16 +6868,16 @@
         <v>44004</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C106" s="5">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="D106" s="5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E106" s="6">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -6851,16 +6885,16 @@
         <v>44005</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C107" s="8">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="D107" s="8">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E107" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -6868,16 +6902,16 @@
         <v>44006</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C108" s="5">
-        <v>145</v>
+        <v>40</v>
       </c>
       <c r="D108" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E108" s="6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -6885,16 +6919,16 @@
         <v>44007</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C109" s="8">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D109" s="8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E109" s="9">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -6902,16 +6936,16 @@
         <v>44008</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C110" s="5">
-        <v>263</v>
+        <v>54</v>
       </c>
       <c r="D110" s="5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E110" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -6919,16 +6953,16 @@
         <v>44009</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C111" s="8">
-        <v>183</v>
+        <v>54</v>
       </c>
       <c r="D111" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E111" s="9">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -6936,13 +6970,13 @@
         <v>44010</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C112" s="10">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="D112" s="10">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E112" s="12">
         <v>0</v>
@@ -6953,16 +6987,16 @@
         <v>44011</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C113" s="11">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D113">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E113" s="13">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -6970,13 +7004,13 @@
         <v>44012</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C114" s="10">
-        <v>139</v>
+        <v>63</v>
       </c>
       <c r="D114">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E114" s="12">
         <v>0</v>
@@ -6987,16 +7021,16 @@
         <v>44013</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C115" s="11">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="D115">
-        <v>19</v>
-      </c>
-      <c r="E115" s="12">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="E115" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -7004,16 +7038,16 @@
         <v>44014</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C116" s="10">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="D116">
-        <v>12</v>
-      </c>
-      <c r="E116" s="13">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="E116" s="12">
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -7021,16 +7055,16 @@
         <v>44015</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C117" s="11">
-        <v>253</v>
+        <v>41</v>
       </c>
       <c r="D117">
-        <v>14</v>
-      </c>
-      <c r="E117" s="12">
-        <v>26</v>
+        <v>5</v>
+      </c>
+      <c r="E117" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -7038,254 +7072,271 @@
         <v>44016</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C118" s="10">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D118">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E118" s="12">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="14">
         <v>44017</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>2</v>
+      <c r="B119" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C119" s="11">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D119">
-        <v>20</v>
-      </c>
-      <c r="E119" s="12">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="E119" s="13">
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="14">
         <v>44018</v>
       </c>
-      <c r="B120" s="8" t="s">
-        <v>2</v>
+      <c r="B120" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C120" s="10">
-        <v>230</v>
+        <v>33</v>
       </c>
       <c r="D120">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E120" s="12">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="14">
         <v>44019</v>
       </c>
-      <c r="B121" s="8" t="s">
-        <v>2</v>
+      <c r="B121" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C121" s="11">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D121">
-        <v>12</v>
-      </c>
-      <c r="E121" s="12">
-        <v>28</v>
+        <v>4</v>
+      </c>
+      <c r="E121" s="13">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="14">
         <v>44020</v>
       </c>
-      <c r="B122" s="8" t="s">
-        <v>2</v>
+      <c r="B122" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C122">
-        <v>143</v>
+        <v>31</v>
       </c>
       <c r="D122">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E122">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="14">
         <v>44021</v>
       </c>
-      <c r="B123" s="8" t="s">
-        <v>2</v>
+      <c r="B123" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C123">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="D123">
-        <v>15</v>
-      </c>
-      <c r="E123" s="10">
-        <v>29</v>
+        <v>2</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="14">
         <v>44022</v>
       </c>
-      <c r="B124" s="8" t="s">
-        <v>2</v>
+      <c r="B124" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C124">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="D124">
-        <v>19</v>
-      </c>
-      <c r="E124" s="10">
-        <v>31</v>
+        <v>4</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="14">
         <v>44023</v>
       </c>
-      <c r="B125" s="8" t="s">
-        <v>2</v>
+      <c r="B125" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C125">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="D125">
-        <v>19</v>
-      </c>
-      <c r="E125" s="10">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="E125">
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="14">
         <v>44024</v>
       </c>
-      <c r="B126" s="8" t="s">
-        <v>2</v>
+      <c r="B126" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C126">
-        <v>174</v>
+        <v>34</v>
       </c>
       <c r="D126">
-        <v>20</v>
-      </c>
-      <c r="E126" s="10">
-        <v>58</v>
+        <v>2</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="14">
         <v>44025</v>
       </c>
-      <c r="B127" s="8" t="s">
-        <v>2</v>
+      <c r="B127" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C127">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>13</v>
-      </c>
-      <c r="E127" s="10">
-        <v>67</v>
+        <v>0</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="14">
         <v>44026</v>
       </c>
-      <c r="B128" s="8" t="s">
-        <v>2</v>
+      <c r="B128" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C128">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="D128">
-        <v>14</v>
-      </c>
-      <c r="E128" s="10">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="14">
         <v>44027</v>
       </c>
-      <c r="B129" s="8" t="s">
-        <v>2</v>
+      <c r="B129" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C129">
-        <v>276</v>
+        <v>48</v>
       </c>
       <c r="D129">
-        <v>10</v>
-      </c>
-      <c r="E129" s="10">
-        <v>84</v>
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="14">
         <v>44028</v>
       </c>
-      <c r="B130" s="8" t="s">
-        <v>2</v>
+      <c r="B130" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C130">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D130">
-        <v>15</v>
-      </c>
-      <c r="E130" s="10">
-        <v>75</v>
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="14">
         <v>44029</v>
       </c>
-      <c r="B131" s="8" t="s">
-        <v>2</v>
+      <c r="B131" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C131">
-        <v>119</v>
+        <v>46</v>
       </c>
       <c r="D131">
-        <v>16</v>
-      </c>
-      <c r="E131" s="10">
-        <v>212</v>
+        <v>2</v>
+      </c>
+      <c r="E131">
+        <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="14">
         <v>44030</v>
       </c>
-      <c r="B132" s="8" t="s">
-        <v>2</v>
+      <c r="B132" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C132">
-        <v>232</v>
+        <v>52</v>
       </c>
       <c r="D132">
-        <v>15</v>
-      </c>
-      <c r="E132" s="10">
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="E132">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133">
+        <v>17</v>
+      </c>
+      <c r="D133">
+        <v>5</v>
+      </c>
+      <c r="E133">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -7295,10 +7346,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9547,6 +9598,23 @@
         <v>38</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C133">
+        <v>733</v>
+      </c>
+      <c r="D133">
+        <v>5</v>
+      </c>
+      <c r="E133">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9554,10 +9622,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11806,6 +11874,23 @@
         <v>32</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C133">
+        <v>34</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11813,10 +11898,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14065,6 +14150,23 @@
         <v>21</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133">
+        <v>26</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14072,10 +14174,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16324,6 +16426,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C133">
+        <v>75</v>
+      </c>
+      <c r="D133">
+        <v>2</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16331,10 +16450,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
     <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133:E133"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18583,6 +18702,23 @@
         <v>119</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C133">
+        <v>270</v>
+      </c>
+      <c r="D133">
+        <v>17</v>
+      </c>
+      <c r="E133">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18590,10 +18726,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E132"/>
+  <dimension ref="A1:E133"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="E133" sqref="C133:E133"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20845,6 +20981,23 @@
         <v>29</v>
       </c>
     </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="14">
+        <v>44031</v>
+      </c>
+      <c r="B133" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133">
+        <v>136</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 27 julio 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D371EFD8-77A2-43D0-B518-486AE58ED3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2630D36-3C01-464A-9A92-435DF03A2A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="600" windowWidth="12405" windowHeight="7935" firstSheet="1" activeTab="7" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="11355" yWindow="255" windowWidth="12405" windowHeight="7935" firstSheet="1" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,6 +2804,125 @@
         <v>2</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135">
+        <v>39</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136">
+        <v>10</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137">
+        <v>20</v>
+      </c>
+      <c r="D137">
+        <v>3</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138">
+        <v>83</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139">
+        <v>13</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="4">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141">
+        <v>5</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="E141">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2811,10 +2930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E135" sqref="E135"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5097,6 +5216,125 @@
         <v>94</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135">
+        <v>168</v>
+      </c>
+      <c r="D135">
+        <v>14</v>
+      </c>
+      <c r="E135" s="10">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C136">
+        <v>193</v>
+      </c>
+      <c r="D136">
+        <v>14</v>
+      </c>
+      <c r="E136" s="10">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C137">
+        <v>160</v>
+      </c>
+      <c r="D137">
+        <v>15</v>
+      </c>
+      <c r="E137" s="10">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C138">
+        <v>258</v>
+      </c>
+      <c r="D138">
+        <v>14</v>
+      </c>
+      <c r="E138" s="10">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C139">
+        <v>115</v>
+      </c>
+      <c r="D139">
+        <v>16</v>
+      </c>
+      <c r="E139" s="10">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C140">
+        <v>124</v>
+      </c>
+      <c r="D140">
+        <v>12</v>
+      </c>
+      <c r="E140" s="10">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C141">
+        <v>560</v>
+      </c>
+      <c r="D141">
+        <v>20</v>
+      </c>
+      <c r="E141" s="10">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5104,10 +5342,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7390,6 +7628,125 @@
         <v>2</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135">
+        <v>25</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C136">
+        <v>36</v>
+      </c>
+      <c r="D136">
+        <v>10</v>
+      </c>
+      <c r="E136">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137">
+        <v>38</v>
+      </c>
+      <c r="D137">
+        <v>9</v>
+      </c>
+      <c r="E137">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C138">
+        <v>71</v>
+      </c>
+      <c r="D138">
+        <v>8</v>
+      </c>
+      <c r="E138">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139">
+        <v>19</v>
+      </c>
+      <c r="D139">
+        <v>3</v>
+      </c>
+      <c r="E139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
+      </c>
+      <c r="D140">
+        <v>7</v>
+      </c>
+      <c r="E140">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141">
+        <v>60</v>
+      </c>
+      <c r="D141">
+        <v>5</v>
+      </c>
+      <c r="E141">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7397,10 +7754,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9683,6 +10040,125 @@
         <v>24</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <v>431</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+      <c r="E135">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C136">
+        <v>788</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C137">
+        <v>534</v>
+      </c>
+      <c r="D137">
+        <v>9</v>
+      </c>
+      <c r="E137">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C138">
+        <v>330</v>
+      </c>
+      <c r="D138">
+        <v>22</v>
+      </c>
+      <c r="E138">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C139">
+        <v>1098</v>
+      </c>
+      <c r="D139">
+        <v>17</v>
+      </c>
+      <c r="E139">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C140">
+        <v>409</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C141">
+        <v>623</v>
+      </c>
+      <c r="D141">
+        <v>7</v>
+      </c>
+      <c r="E141">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9690,10 +10166,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11976,6 +12452,125 @@
         <v>22</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135">
+        <v>102</v>
+      </c>
+      <c r="D135">
+        <v>7</v>
+      </c>
+      <c r="E135">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C136">
+        <v>85</v>
+      </c>
+      <c r="D136">
+        <v>8</v>
+      </c>
+      <c r="E136">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137">
+        <v>75</v>
+      </c>
+      <c r="D137">
+        <v>6</v>
+      </c>
+      <c r="E137">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138">
+        <v>51</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139">
+        <v>100</v>
+      </c>
+      <c r="D139">
+        <v>5</v>
+      </c>
+      <c r="E139">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140">
+        <v>99</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+      <c r="E140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C141">
+        <v>66</v>
+      </c>
+      <c r="D141">
+        <v>9</v>
+      </c>
+      <c r="E141">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11983,10 +12578,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14269,6 +14864,125 @@
         <v>8</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>5</v>
+      </c>
+      <c r="E135">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <v>87</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="E136">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <v>11</v>
+      </c>
+      <c r="D137">
+        <v>9</v>
+      </c>
+      <c r="E137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <v>51</v>
+      </c>
+      <c r="D138">
+        <v>3</v>
+      </c>
+      <c r="E138">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>3</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141">
+        <v>6</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14276,10 +14990,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16562,6 +17276,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136">
+        <v>61</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C137">
+        <v>17</v>
+      </c>
+      <c r="D137">
+        <v>10</v>
+      </c>
+      <c r="E137">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>119</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C139">
+        <v>5</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>46</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
+      </c>
+      <c r="E140">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C141">
+        <v>7</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16569,10 +17402,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C134" sqref="C2:C134"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134:E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18855,6 +19688,125 @@
         <v>148</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135">
+        <v>578</v>
+      </c>
+      <c r="D135">
+        <v>21</v>
+      </c>
+      <c r="E135">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136">
+        <v>513</v>
+      </c>
+      <c r="D136">
+        <v>20</v>
+      </c>
+      <c r="E136">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137">
+        <v>256</v>
+      </c>
+      <c r="D137">
+        <v>17</v>
+      </c>
+      <c r="E137">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138">
+        <v>190</v>
+      </c>
+      <c r="D138">
+        <v>17</v>
+      </c>
+      <c r="E138">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139">
+        <v>292</v>
+      </c>
+      <c r="D139">
+        <v>20</v>
+      </c>
+      <c r="E139">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C140">
+        <v>234</v>
+      </c>
+      <c r="D140">
+        <v>20</v>
+      </c>
+      <c r="E140">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C141">
+        <v>281</v>
+      </c>
+      <c r="D141">
+        <v>19</v>
+      </c>
+      <c r="E141">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18862,10 +19814,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="D128" sqref="D128"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21151,6 +22103,125 @@
         <v>22</v>
       </c>
     </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="14">
+        <v>44033</v>
+      </c>
+      <c r="B135" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C135">
+        <v>22</v>
+      </c>
+      <c r="D135">
+        <v>4</v>
+      </c>
+      <c r="E135">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="14">
+        <v>44034</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136">
+        <v>5</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="14">
+        <v>44035</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137">
+        <v>6</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="14">
+        <v>44036</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C138">
+        <v>51</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="14">
+        <v>44037</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C139">
+        <v>180</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="14">
+        <v>44038</v>
+      </c>
+      <c r="B140" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>225</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+      <c r="E140">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="14">
+        <v>44039</v>
+      </c>
+      <c r="B141" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C141">
+        <v>144</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 29 julio 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2630D36-3C01-464A-9A92-435DF03A2A50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E69351C-8830-40C9-B5DA-CC45B668CD5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="255" windowWidth="12405" windowHeight="7935" firstSheet="1" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="12045" yWindow="945" windowWidth="12405" windowHeight="7935" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="F141" sqref="F141"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2923,6 +2923,40 @@
         <v>11</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="4">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142">
+        <v>20</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="4">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2930,10 +2964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView topLeftCell="C120" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5335,6 +5369,40 @@
         <v>97</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C142">
+        <v>206</v>
+      </c>
+      <c r="D142">
+        <v>19</v>
+      </c>
+      <c r="E142" s="10">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C143">
+        <v>100</v>
+      </c>
+      <c r="D143">
+        <v>12</v>
+      </c>
+      <c r="E143" s="10">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5342,10 +5410,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7747,6 +7815,40 @@
         <v>41</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142">
+        <v>27</v>
+      </c>
+      <c r="D142">
+        <v>11</v>
+      </c>
+      <c r="E142">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143">
+        <v>23</v>
+      </c>
+      <c r="D143">
+        <v>4</v>
+      </c>
+      <c r="E143">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7754,10 +7856,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10159,6 +10261,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C142">
+        <v>215</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C143">
+        <v>364</v>
+      </c>
+      <c r="D143">
+        <v>28</v>
+      </c>
+      <c r="E143">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10166,10 +10302,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12571,6 +12707,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C142">
+        <v>37</v>
+      </c>
+      <c r="D142">
+        <v>3</v>
+      </c>
+      <c r="E142">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C143">
+        <v>54</v>
+      </c>
+      <c r="D143">
+        <v>4</v>
+      </c>
+      <c r="E143">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12578,10 +12748,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14983,6 +15153,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142">
+        <v>2</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>23</v>
+      </c>
+      <c r="D143">
+        <v>3</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14990,10 +15194,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="F140" sqref="F140"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17395,6 +17599,40 @@
         <v>26</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142">
+        <v>15</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C143">
+        <v>6</v>
+      </c>
+      <c r="D143">
+        <v>5</v>
+      </c>
+      <c r="E143">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17402,10 +17640,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134:E141"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144:F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19807,6 +20045,40 @@
         <v>72</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C142">
+        <v>431</v>
+      </c>
+      <c r="D142">
+        <v>33</v>
+      </c>
+      <c r="E142">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C143">
+        <v>466</v>
+      </c>
+      <c r="D143">
+        <v>29</v>
+      </c>
+      <c r="E143">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19814,10 +20086,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E141"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A140" sqref="A140"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22222,6 +22494,40 @@
         <v>40</v>
       </c>
     </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="14">
+        <v>44040</v>
+      </c>
+      <c r="B142" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C142">
+        <v>193</v>
+      </c>
+      <c r="D142">
+        <v>3</v>
+      </c>
+      <c r="E142">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="14">
+        <v>44041</v>
+      </c>
+      <c r="B143" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143">
+        <v>161</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+      <c r="E143">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 9 de agosto de 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE9C97A-6C25-4B76-AE9A-58DCBAFB9255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33C113-50E4-4446-A409-2E52DC81C359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="810" windowWidth="12405" windowHeight="10080" firstSheet="1" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="26160" windowHeight="11760" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1359" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -515,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,6 +3019,125 @@
         <v>8</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="4">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148">
+        <v>19</v>
+      </c>
+      <c r="D148">
+        <v>2</v>
+      </c>
+      <c r="E148">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="4">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149">
+        <v>31</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="4">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150">
+        <v>28</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+      <c r="E150">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151">
+        <v>32</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
+      </c>
+      <c r="E151">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="4">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152">
+        <v>31</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="4">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153">
+        <v>17</v>
+      </c>
+      <c r="D153">
+        <v>2</v>
+      </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="4">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154">
+        <v>12</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3032,10 +3145,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5539,6 +5652,125 @@
         <v>86</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C148">
+        <v>189</v>
+      </c>
+      <c r="D148">
+        <v>15</v>
+      </c>
+      <c r="E148" s="10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C149">
+        <v>216</v>
+      </c>
+      <c r="D149">
+        <v>17</v>
+      </c>
+      <c r="E149" s="10">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C150">
+        <v>182</v>
+      </c>
+      <c r="D150">
+        <v>15</v>
+      </c>
+      <c r="E150" s="10">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C151">
+        <v>96</v>
+      </c>
+      <c r="D151">
+        <v>14</v>
+      </c>
+      <c r="E151" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C152">
+        <v>83</v>
+      </c>
+      <c r="D152">
+        <v>12</v>
+      </c>
+      <c r="E152" s="10">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C153">
+        <v>43</v>
+      </c>
+      <c r="D153">
+        <v>10</v>
+      </c>
+      <c r="E153" s="10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154">
+        <v>151</v>
+      </c>
+      <c r="D154">
+        <v>5</v>
+      </c>
+      <c r="E154" s="10">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5546,10 +5778,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8053,6 +8285,125 @@
         <v>7</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C148">
+        <v>58</v>
+      </c>
+      <c r="D148">
+        <v>9</v>
+      </c>
+      <c r="E148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149">
+        <v>62</v>
+      </c>
+      <c r="D149">
+        <v>4</v>
+      </c>
+      <c r="E149">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C150">
+        <v>76</v>
+      </c>
+      <c r="D150">
+        <v>6</v>
+      </c>
+      <c r="E150">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151">
+        <v>99</v>
+      </c>
+      <c r="D151">
+        <v>9</v>
+      </c>
+      <c r="E151">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C152">
+        <v>126</v>
+      </c>
+      <c r="D152">
+        <v>13</v>
+      </c>
+      <c r="E152">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153">
+        <v>99</v>
+      </c>
+      <c r="D153">
+        <v>13</v>
+      </c>
+      <c r="E153">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C154">
+        <v>51</v>
+      </c>
+      <c r="D154">
+        <v>8</v>
+      </c>
+      <c r="E154">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8060,10 +8411,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10567,6 +10918,125 @@
         <v>18</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C148">
+        <v>876</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149">
+        <v>416</v>
+      </c>
+      <c r="D149">
+        <v>21</v>
+      </c>
+      <c r="E149">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C150">
+        <v>909</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C151">
+        <v>551</v>
+      </c>
+      <c r="D151">
+        <v>16</v>
+      </c>
+      <c r="E151">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C152">
+        <v>906</v>
+      </c>
+      <c r="D152">
+        <v>6</v>
+      </c>
+      <c r="E152">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C153">
+        <v>624</v>
+      </c>
+      <c r="D153">
+        <v>9</v>
+      </c>
+      <c r="E153">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C154">
+        <v>501</v>
+      </c>
+      <c r="D154">
+        <v>10</v>
+      </c>
+      <c r="E154">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10574,10 +11044,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="D153" sqref="D153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13081,6 +13551,125 @@
         <v>25</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148">
+        <v>48</v>
+      </c>
+      <c r="D148">
+        <v>4</v>
+      </c>
+      <c r="E148">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149">
+        <v>149</v>
+      </c>
+      <c r="D149">
+        <v>6</v>
+      </c>
+      <c r="E149">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150">
+        <v>70</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+      <c r="E150">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151">
+        <v>67</v>
+      </c>
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152">
+        <v>12</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153">
+        <v>78</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154">
+        <v>21</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13088,10 +13677,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+    <sheetView topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15595,6 +16184,125 @@
         <v>8</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="D148">
+        <v>6</v>
+      </c>
+      <c r="E148">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>28</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>36</v>
+      </c>
+      <c r="D150">
+        <v>5</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>22</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C152">
+        <v>32</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153">
+        <v>38</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154">
+        <v>35</v>
+      </c>
+      <c r="D154">
+        <v>3</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15602,10 +16310,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="E146" sqref="E146"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18109,6 +18817,125 @@
         <v>1</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148">
+        <v>51</v>
+      </c>
+      <c r="D148">
+        <v>8</v>
+      </c>
+      <c r="E148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C149">
+        <v>43</v>
+      </c>
+      <c r="D149">
+        <v>3</v>
+      </c>
+      <c r="E149">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150">
+        <v>77</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C151">
+        <v>13</v>
+      </c>
+      <c r="D151">
+        <v>2</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152">
+        <v>32</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C153">
+        <v>28</v>
+      </c>
+      <c r="D153">
+        <v>5</v>
+      </c>
+      <c r="E153">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154">
+        <v>40</v>
+      </c>
+      <c r="D154">
+        <v>4</v>
+      </c>
+      <c r="E154">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18116,10 +18943,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E144" sqref="E144"/>
+      <selection activeCell="F154" sqref="F154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20623,6 +21450,125 @@
         <v>12</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C148">
+        <v>324</v>
+      </c>
+      <c r="D148">
+        <v>27</v>
+      </c>
+      <c r="E148">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C149">
+        <v>463</v>
+      </c>
+      <c r="D149">
+        <v>35</v>
+      </c>
+      <c r="E149">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C150">
+        <v>322</v>
+      </c>
+      <c r="D150">
+        <v>31</v>
+      </c>
+      <c r="E150">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C151">
+        <v>378</v>
+      </c>
+      <c r="D151">
+        <v>29</v>
+      </c>
+      <c r="E151">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C152">
+        <v>229</v>
+      </c>
+      <c r="D152">
+        <v>19</v>
+      </c>
+      <c r="E152">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C153">
+        <v>236</v>
+      </c>
+      <c r="D153">
+        <v>18</v>
+      </c>
+      <c r="E153">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C154">
+        <v>133</v>
+      </c>
+      <c r="D154">
+        <v>21</v>
+      </c>
+      <c r="E154">
+        <v>563</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20630,10 +21576,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E147"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="C147" sqref="C147"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23140,6 +24086,125 @@
         <v>23</v>
       </c>
     </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="14">
+        <v>44046</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C148">
+        <v>125</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+      <c r="E148">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="14">
+        <v>44047</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149">
+        <v>107</v>
+      </c>
+      <c r="D149">
+        <v>5</v>
+      </c>
+      <c r="E149">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="14">
+        <v>44048</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150">
+        <v>80</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="14">
+        <v>44049</v>
+      </c>
+      <c r="B151" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C151">
+        <v>24</v>
+      </c>
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="14">
+        <v>44050</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C152">
+        <v>17</v>
+      </c>
+      <c r="D152">
+        <v>5</v>
+      </c>
+      <c r="E152">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="14">
+        <v>44051</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="D153">
+        <v>5</v>
+      </c>
+      <c r="E153">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="14">
+        <v>44052</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>2</v>
+      </c>
+      <c r="E154">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 16 de agosto de 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD33C113-50E4-4446-A409-2E52DC81C359}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8BDD54-2B7B-4B90-9A54-02847EB45ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="26160" windowHeight="11760" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3138,6 +3138,129 @@
         <v>4</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="4">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C155">
+        <v>47</v>
+      </c>
+      <c r="D155">
+        <v>3</v>
+      </c>
+      <c r="E155">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="4">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>85</v>
+      </c>
+      <c r="D156">
+        <v>4</v>
+      </c>
+      <c r="E156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157">
+        <v>9</v>
+      </c>
+      <c r="D157">
+        <v>3</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="4">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158">
+        <v>24</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="4">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+      <c r="E159">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="4">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160">
+        <v>3</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="4">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="4"/>
+      <c r="B162" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3145,10 +3268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E162"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5771,6 +5894,128 @@
         <v>147</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C155">
+        <v>136</v>
+      </c>
+      <c r="D155">
+        <v>5</v>
+      </c>
+      <c r="E155" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156">
+        <v>123</v>
+      </c>
+      <c r="D156">
+        <v>5</v>
+      </c>
+      <c r="E156" s="10">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C157">
+        <v>145</v>
+      </c>
+      <c r="D157">
+        <v>5</v>
+      </c>
+      <c r="E157" s="10">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C158">
+        <v>84</v>
+      </c>
+      <c r="D158">
+        <v>8</v>
+      </c>
+      <c r="E158" s="10">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C159">
+        <v>185</v>
+      </c>
+      <c r="D159">
+        <v>7</v>
+      </c>
+      <c r="E159" s="10">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C160">
+        <v>87</v>
+      </c>
+      <c r="D160">
+        <v>6</v>
+      </c>
+      <c r="E160" s="10">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C161">
+        <v>13</v>
+      </c>
+      <c r="D161">
+        <v>10</v>
+      </c>
+      <c r="E161" s="10">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E162" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5778,10 +6023,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8404,6 +8649,125 @@
         <v>63</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155">
+        <v>125</v>
+      </c>
+      <c r="D155">
+        <v>10</v>
+      </c>
+      <c r="E155">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156">
+        <v>141</v>
+      </c>
+      <c r="D156">
+        <v>11</v>
+      </c>
+      <c r="E156">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157">
+        <v>149</v>
+      </c>
+      <c r="D157">
+        <v>10</v>
+      </c>
+      <c r="E157">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C158">
+        <v>169</v>
+      </c>
+      <c r="D158">
+        <v>11</v>
+      </c>
+      <c r="E158">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159">
+        <v>181</v>
+      </c>
+      <c r="D159">
+        <v>13</v>
+      </c>
+      <c r="E159">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C160">
+        <v>146</v>
+      </c>
+      <c r="D160">
+        <v>6</v>
+      </c>
+      <c r="E160">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161">
+        <v>185</v>
+      </c>
+      <c r="D161">
+        <v>7</v>
+      </c>
+      <c r="E161">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8411,10 +8775,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="E153" sqref="E153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11037,6 +11401,125 @@
         <v>81</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C155">
+        <v>716</v>
+      </c>
+      <c r="D155">
+        <v>7</v>
+      </c>
+      <c r="E155">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C156">
+        <v>586</v>
+      </c>
+      <c r="D156">
+        <v>4</v>
+      </c>
+      <c r="E156">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C157">
+        <v>813</v>
+      </c>
+      <c r="D157">
+        <v>19</v>
+      </c>
+      <c r="E157">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C158">
+        <v>424</v>
+      </c>
+      <c r="D158">
+        <v>12</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C159">
+        <v>457</v>
+      </c>
+      <c r="D159">
+        <v>12</v>
+      </c>
+      <c r="E159">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C160">
+        <v>520</v>
+      </c>
+      <c r="D160">
+        <v>24</v>
+      </c>
+      <c r="E160">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C161">
+        <v>654</v>
+      </c>
+      <c r="D161">
+        <v>15</v>
+      </c>
+      <c r="E161">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11044,10 +11527,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D153" sqref="D153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13670,6 +14153,125 @@
         <v>2</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155">
+        <v>12</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156">
+        <v>43</v>
+      </c>
+      <c r="D156">
+        <v>2</v>
+      </c>
+      <c r="E156">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157">
+        <v>21</v>
+      </c>
+      <c r="D157">
+        <v>2</v>
+      </c>
+      <c r="E157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158">
+        <v>13</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C159">
+        <v>10</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C160">
+        <v>18</v>
+      </c>
+      <c r="D160">
+        <v>2</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161">
+        <v>14</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13677,10 +14279,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="C153" sqref="C153"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16303,6 +16905,125 @@
         <v>0</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155">
+        <v>34</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156">
+        <v>54</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157">
+        <v>56</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C158">
+        <v>38</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159">
+        <v>48</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C160">
+        <v>58</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161">
+        <v>49</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16310,10 +17031,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18936,6 +19657,125 @@
         <v>6</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C155">
+        <v>81</v>
+      </c>
+      <c r="D155">
+        <v>35</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156">
+        <v>291</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157">
+        <v>120</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158">
+        <v>256</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159">
+        <v>235</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160">
+        <v>194</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C161">
+        <v>116</v>
+      </c>
+      <c r="D161">
+        <v>3</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18943,10 +19783,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="D161" sqref="D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21569,6 +22409,125 @@
         <v>563</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155">
+        <v>335</v>
+      </c>
+      <c r="D155">
+        <v>29</v>
+      </c>
+      <c r="E155">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C156">
+        <v>207</v>
+      </c>
+      <c r="D156">
+        <v>18</v>
+      </c>
+      <c r="E156">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C157">
+        <v>232</v>
+      </c>
+      <c r="D157">
+        <v>21</v>
+      </c>
+      <c r="E157">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C158">
+        <v>185</v>
+      </c>
+      <c r="D158">
+        <v>15</v>
+      </c>
+      <c r="E158">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C159">
+        <v>171</v>
+      </c>
+      <c r="D159">
+        <v>13</v>
+      </c>
+      <c r="E159">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160">
+        <v>114</v>
+      </c>
+      <c r="D160">
+        <v>19</v>
+      </c>
+      <c r="E160">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161">
+        <v>115</v>
+      </c>
+      <c r="D161">
+        <v>15</v>
+      </c>
+      <c r="E161">
+        <v>387</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21576,10 +22535,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E154"/>
+  <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24205,6 +25164,125 @@
         <v>38</v>
       </c>
     </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="14">
+        <v>44053</v>
+      </c>
+      <c r="B155" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C155">
+        <v>150</v>
+      </c>
+      <c r="D155">
+        <v>3</v>
+      </c>
+      <c r="E155">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="14">
+        <v>44054</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156">
+        <v>163</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="14">
+        <v>44055</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <v>198</v>
+      </c>
+      <c r="D157">
+        <v>5</v>
+      </c>
+      <c r="E157">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="14">
+        <v>44056</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C158">
+        <v>195</v>
+      </c>
+      <c r="D158">
+        <v>3</v>
+      </c>
+      <c r="E158">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="14">
+        <v>44057</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C159">
+        <v>204</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+      <c r="E159">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="14">
+        <v>44058</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C160">
+        <v>56</v>
+      </c>
+      <c r="D160">
+        <v>2</v>
+      </c>
+      <c r="E160">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="14">
+        <v>44059</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C161">
+        <v>52</v>
+      </c>
+      <c r="D161">
+        <v>3</v>
+      </c>
+      <c r="E161">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actulizado al 18 de agosto 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8BDD54-2B7B-4B90-9A54-02847EB45ED1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F7053F-C9D6-4332-A367-BCB603684D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,8 +3258,38 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="4"/>
-      <c r="B162" s="8"/>
+      <c r="A162" s="4">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162">
+        <v>14</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="4">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163">
+        <v>51</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3268,10 +3298,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6014,7 +6044,38 @@
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E162" s="10"/>
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C162">
+        <v>52</v>
+      </c>
+      <c r="D162">
+        <v>7</v>
+      </c>
+      <c r="E162" s="10">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C163">
+        <v>80</v>
+      </c>
+      <c r="D163">
+        <v>8</v>
+      </c>
+      <c r="E163" s="10">
+        <v>320</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6023,10 +6084,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E162" sqref="E162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8768,6 +8829,40 @@
         <v>23</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C162">
+        <v>177</v>
+      </c>
+      <c r="D162">
+        <v>8</v>
+      </c>
+      <c r="E162">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163">
+        <v>162</v>
+      </c>
+      <c r="D163">
+        <v>9</v>
+      </c>
+      <c r="E163">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8775,10 +8870,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11520,6 +11615,48 @@
         <v>170</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C162">
+        <v>276</v>
+      </c>
+      <c r="D162">
+        <v>15</v>
+      </c>
+      <c r="E162">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163">
+        <v>243</v>
+      </c>
+      <c r="D163">
+        <v>8</v>
+      </c>
+      <c r="E163">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14"/>
+      <c r="B164" s="8"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14"/>
+      <c r="B165" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11527,10 +11664,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="F162" sqref="F162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14272,6 +14409,40 @@
         <v>4</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162">
+        <v>14</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C163">
+        <v>16</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14279,10 +14450,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17024,6 +17195,40 @@
         <v>3</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C162">
+        <v>9</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163">
+        <v>53</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17031,10 +17236,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19776,6 +19981,40 @@
         <v>2</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>138</v>
+      </c>
+      <c r="D162">
+        <v>14</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C163">
+        <v>861</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+      <c r="E163">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19783,10 +20022,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="D161" sqref="D161"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="C163" sqref="C163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22528,6 +22767,40 @@
         <v>387</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162">
+        <v>95</v>
+      </c>
+      <c r="D162">
+        <v>16</v>
+      </c>
+      <c r="E162">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C163">
+        <v>69</v>
+      </c>
+      <c r="D163">
+        <v>15</v>
+      </c>
+      <c r="E163">
+        <v>479</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22535,10 +22808,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25283,6 +25556,40 @@
         <v>5</v>
       </c>
     </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="14">
+        <v>44060</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <v>104</v>
+      </c>
+      <c r="D162">
+        <v>4</v>
+      </c>
+      <c r="E162">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="14">
+        <v>44061</v>
+      </c>
+      <c r="B163" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C163">
+        <v>261</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+      <c r="E163">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizado 19 de agosto 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14F7053F-C9D6-4332-A367-BCB603684D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A45F27-CF2D-4E42-8E84-B5BDB33F1F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="3" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3291,6 +3291,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="4">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164">
+        <v>71</v>
+      </c>
+      <c r="D164">
+        <v>2</v>
+      </c>
+      <c r="E164">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3298,10 +3315,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6077,6 +6094,23 @@
         <v>320</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C164">
+        <v>72</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="E164" s="10">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6084,10 +6118,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E162" sqref="E162"/>
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8861,6 +8895,23 @@
       </c>
       <c r="E163">
         <v>72</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164">
+        <v>107</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="E164">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -8872,8 +8923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11650,8 +11701,21 @@
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="14"/>
-      <c r="B164" s="8"/>
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C164">
+        <v>805</v>
+      </c>
+      <c r="D164">
+        <v>16</v>
+      </c>
+      <c r="E164">
+        <v>147</v>
+      </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
@@ -11664,10 +11728,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14443,6 +14507,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C164">
+        <v>68</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14450,10 +14531,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="D163" sqref="D163"/>
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17229,6 +17310,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <v>53</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17236,10 +17334,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+      <selection activeCell="E164" sqref="E164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20015,6 +20113,23 @@
         <v>91</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C164">
+        <v>268</v>
+      </c>
+      <c r="D164">
+        <v>5</v>
+      </c>
+      <c r="E164">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20022,10 +20137,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="C163" sqref="C163"/>
+      <selection activeCell="F164" sqref="F164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22801,6 +22916,23 @@
         <v>479</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C164">
+        <v>282</v>
+      </c>
+      <c r="D164">
+        <v>25</v>
+      </c>
+      <c r="E164">
+        <v>508</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22808,7 +22940,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E163"/>
+  <dimension ref="A1:E164"/>
   <sheetViews>
     <sheetView topLeftCell="A148" workbookViewId="0">
       <selection activeCell="E164" sqref="E164"/>
@@ -25590,6 +25722,23 @@
         <v>28</v>
       </c>
     </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="14">
+        <v>44062</v>
+      </c>
+      <c r="B164" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C164">
+        <v>305</v>
+      </c>
+      <c r="D164">
+        <v>3</v>
+      </c>
+      <c r="E164">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 20 de agosto de 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A45F27-CF2D-4E42-8E84-B5BDB33F1F17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140C8C9-303E-4432-9D6F-7FCB18990497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="3" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1512" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,6 +3308,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="4">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165">
+        <v>63</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3315,10 +3332,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6111,6 +6128,23 @@
         <v>180</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C165">
+        <v>58</v>
+      </c>
+      <c r="D165">
+        <v>7</v>
+      </c>
+      <c r="E165" s="10">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6118,10 +6152,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8912,6 +8946,23 @@
       </c>
       <c r="E164">
         <v>76</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165">
+        <v>89</v>
+      </c>
+      <c r="D165">
+        <v>5</v>
+      </c>
+      <c r="E165">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -8923,8 +8974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
   <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="D167" sqref="D167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11718,8 +11769,21 @@
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="14"/>
-      <c r="B165" s="8"/>
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C165">
+        <v>206</v>
+      </c>
+      <c r="D165">
+        <v>14</v>
+      </c>
+      <c r="E165">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11728,10 +11792,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14524,6 +14588,23 @@
         <v>384</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165">
+        <v>129</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14531,10 +14612,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17327,6 +17408,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C165">
+        <v>55</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17334,10 +17432,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20130,6 +20228,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165">
+        <v>118</v>
+      </c>
+      <c r="D165">
+        <v>7</v>
+      </c>
+      <c r="E165">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20137,10 +20252,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F164" sqref="F164"/>
+      <selection activeCell="F165" sqref="F165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22933,6 +23048,23 @@
         <v>508</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C165">
+        <v>107</v>
+      </c>
+      <c r="D165">
+        <v>29</v>
+      </c>
+      <c r="E165">
+        <v>408</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22940,10 +23072,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E165"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E164" sqref="E164"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25739,6 +25871,23 @@
         <v>32</v>
       </c>
     </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="14">
+        <v>44063</v>
+      </c>
+      <c r="B165" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C165">
+        <v>190</v>
+      </c>
+      <c r="D165">
+        <v>5</v>
+      </c>
+      <c r="E165">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 21 de agosto 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C140C8C9-303E-4432-9D6F-7FCB18990497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66394177-C2DD-4D9C-BDBC-68D2E9868245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="0" windowWidth="17670" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="10695" yWindow="390" windowWidth="12870" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3325,6 +3325,23 @@
         <v>76</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="4">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166">
+        <v>82</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3332,10 +3349,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6145,6 +6162,23 @@
         <v>270</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C166">
+        <v>68</v>
+      </c>
+      <c r="D166">
+        <v>6</v>
+      </c>
+      <c r="E166" s="10">
+        <v>251</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6152,10 +6186,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8965,6 +8999,23 @@
         <v>56</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C166">
+        <v>78</v>
+      </c>
+      <c r="D166">
+        <v>10</v>
+      </c>
+      <c r="E166">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8972,10 +9023,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="D167" sqref="D167"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11785,6 +11836,23 @@
         <v>63</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166">
+        <v>465</v>
+      </c>
+      <c r="D166">
+        <v>14</v>
+      </c>
+      <c r="E166">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11792,10 +11860,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166:B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14605,6 +14673,23 @@
         <v>208</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166">
+        <v>79</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14612,10 +14697,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17425,6 +17510,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C166">
+        <v>79</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17432,10 +17534,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20245,6 +20347,23 @@
         <v>33</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166">
+        <v>98</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20252,10 +20371,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E166" sqref="E166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23065,6 +23184,23 @@
         <v>408</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C166">
+        <v>144</v>
+      </c>
+      <c r="D166">
+        <v>26</v>
+      </c>
+      <c r="E166">
+        <v>472</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23072,10 +23208,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E165" sqref="E165"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="E167" sqref="E167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25888,6 +26024,23 @@
         <v>32</v>
       </c>
     </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="14">
+        <v>44064</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C166">
+        <v>277</v>
+      </c>
+      <c r="D166">
+        <v>5</v>
+      </c>
+      <c r="E166">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 24 de agosto 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66394177-C2DD-4D9C-BDBC-68D2E9868245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FED11A7-F111-4222-9B9D-ED0822FFD6B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10695" yWindow="390" windowWidth="12870" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="13860" yWindow="45" windowWidth="12870" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,6 +3342,57 @@
         <v>28</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="4">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C167">
+        <v>84</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="4">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168">
+        <v>13</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="4">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169">
+        <v>7</v>
+      </c>
+      <c r="D169">
+        <v>2</v>
+      </c>
+      <c r="E169">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3349,10 +3400,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6179,6 +6230,57 @@
         <v>251</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C167">
+        <v>102</v>
+      </c>
+      <c r="D167">
+        <v>5</v>
+      </c>
+      <c r="E167" s="10">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C168">
+        <v>53</v>
+      </c>
+      <c r="D168">
+        <v>9</v>
+      </c>
+      <c r="E168" s="10">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169">
+        <v>112</v>
+      </c>
+      <c r="D169">
+        <v>8</v>
+      </c>
+      <c r="E169" s="10">
+        <v>195</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6186,10 +6288,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9016,6 +9118,57 @@
         <v>51</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167">
+        <v>115</v>
+      </c>
+      <c r="D167">
+        <v>6</v>
+      </c>
+      <c r="E167">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C168">
+        <v>102</v>
+      </c>
+      <c r="D168">
+        <v>4</v>
+      </c>
+      <c r="E168">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169">
+        <v>67</v>
+      </c>
+      <c r="D169">
+        <v>5</v>
+      </c>
+      <c r="E169">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9023,10 +9176,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11853,6 +12006,57 @@
         <v>153</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C167">
+        <v>214</v>
+      </c>
+      <c r="D167">
+        <v>20</v>
+      </c>
+      <c r="E167">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C168">
+        <v>343</v>
+      </c>
+      <c r="D168">
+        <v>24</v>
+      </c>
+      <c r="E168">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C169">
+        <v>607</v>
+      </c>
+      <c r="D169">
+        <v>17</v>
+      </c>
+      <c r="E169">
+        <v>796</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11860,10 +12064,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166:B166"/>
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14690,6 +14894,57 @@
         <v>31</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C167">
+        <v>61</v>
+      </c>
+      <c r="D167">
+        <v>5</v>
+      </c>
+      <c r="E167">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C168">
+        <v>53</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C169">
+        <v>29</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14697,10 +14952,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17527,6 +17782,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167">
+        <v>22</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C169">
+        <v>9</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17534,10 +17840,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20364,6 +20670,57 @@
         <v>10</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C167">
+        <v>100</v>
+      </c>
+      <c r="D167">
+        <v>3</v>
+      </c>
+      <c r="E167">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C168">
+        <v>35</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C169">
+        <v>61</v>
+      </c>
+      <c r="D169">
+        <v>4</v>
+      </c>
+      <c r="E169">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20371,10 +20728,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23201,6 +23558,57 @@
         <v>472</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C167">
+        <v>173</v>
+      </c>
+      <c r="D167">
+        <v>29</v>
+      </c>
+      <c r="E167">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C168">
+        <v>87</v>
+      </c>
+      <c r="D168">
+        <v>26</v>
+      </c>
+      <c r="E168">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169">
+        <v>64</v>
+      </c>
+      <c r="D169">
+        <v>26</v>
+      </c>
+      <c r="E169">
+        <v>518</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23208,10 +23616,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="E167" sqref="E167"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26041,6 +26449,57 @@
         <v>32</v>
       </c>
     </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="14">
+        <v>44065</v>
+      </c>
+      <c r="B167" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C167">
+        <v>121</v>
+      </c>
+      <c r="D167">
+        <v>7</v>
+      </c>
+      <c r="E167">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="14">
+        <v>44066</v>
+      </c>
+      <c r="B168" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C168">
+        <v>34</v>
+      </c>
+      <c r="D168">
+        <v>2</v>
+      </c>
+      <c r="E168">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="14">
+        <v>44067</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C169">
+        <v>43</v>
+      </c>
+      <c r="D169">
+        <v>6</v>
+      </c>
+      <c r="E169">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 2 de septiembre 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576C2BC0-D9B6-42CE-A727-5E5024967680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AB8918-0F80-41CD-9234-920D8474E1EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="45" windowWidth="12870" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="2445" yWindow="45" windowWidth="23325" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1557" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="E170" sqref="E170"/>
+    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3393,6 +3393,163 @@
         <v>45</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="4">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C170">
+        <v>80</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="4">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171">
+        <v>27</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="4">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C172">
+        <v>53</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="4">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173">
+        <v>63</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="4">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174">
+        <v>19</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="4">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C175">
+        <v>8</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="4">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C176">
+        <v>18</v>
+      </c>
+      <c r="D176">
+        <v>2</v>
+      </c>
+      <c r="E176">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="4">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177">
+        <v>29</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="4">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178">
+        <v>32</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="4"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3400,10 +3557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6281,6 +6438,163 @@
         <v>195</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C170">
+        <v>61</v>
+      </c>
+      <c r="D170">
+        <v>9</v>
+      </c>
+      <c r="E170" s="10">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C171">
+        <v>51</v>
+      </c>
+      <c r="D171">
+        <v>7</v>
+      </c>
+      <c r="E171" s="10">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C172">
+        <v>93</v>
+      </c>
+      <c r="D172">
+        <v>10</v>
+      </c>
+      <c r="E172" s="10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C173">
+        <v>43</v>
+      </c>
+      <c r="D173">
+        <v>8</v>
+      </c>
+      <c r="E173" s="10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C174">
+        <v>86</v>
+      </c>
+      <c r="D174">
+        <v>7</v>
+      </c>
+      <c r="E174" s="10">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C175">
+        <v>7</v>
+      </c>
+      <c r="D175">
+        <v>6</v>
+      </c>
+      <c r="E175" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C176">
+        <v>73</v>
+      </c>
+      <c r="D176">
+        <v>7</v>
+      </c>
+      <c r="E176" s="10">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C177">
+        <v>62</v>
+      </c>
+      <c r="D177">
+        <v>8</v>
+      </c>
+      <c r="E177" s="10">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C178">
+        <v>84</v>
+      </c>
+      <c r="D178">
+        <v>6</v>
+      </c>
+      <c r="E178" s="10">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6288,10 +6602,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9169,6 +9483,163 @@
         <v>53</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C170">
+        <v>81</v>
+      </c>
+      <c r="D170">
+        <v>6</v>
+      </c>
+      <c r="E170">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C171">
+        <v>65</v>
+      </c>
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C172">
+        <v>72</v>
+      </c>
+      <c r="D172">
+        <v>3</v>
+      </c>
+      <c r="E172">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173">
+        <v>101</v>
+      </c>
+      <c r="D173">
+        <v>10</v>
+      </c>
+      <c r="E173">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C174">
+        <v>73</v>
+      </c>
+      <c r="D174">
+        <v>5</v>
+      </c>
+      <c r="E174">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175">
+        <v>36</v>
+      </c>
+      <c r="D175">
+        <v>3</v>
+      </c>
+      <c r="E175">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C176">
+        <v>87</v>
+      </c>
+      <c r="D176">
+        <v>7</v>
+      </c>
+      <c r="E176">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C177">
+        <v>75</v>
+      </c>
+      <c r="D177">
+        <v>5</v>
+      </c>
+      <c r="E177">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C178">
+        <v>65</v>
+      </c>
+      <c r="D178">
+        <v>5</v>
+      </c>
+      <c r="E178">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="14"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9176,10 +9647,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12057,6 +12528,163 @@
         <v>796</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C170">
+        <v>214</v>
+      </c>
+      <c r="D170">
+        <v>22</v>
+      </c>
+      <c r="E170">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171">
+        <v>349</v>
+      </c>
+      <c r="D171">
+        <v>23</v>
+      </c>
+      <c r="E171">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C172">
+        <v>353</v>
+      </c>
+      <c r="D172">
+        <v>18</v>
+      </c>
+      <c r="E172">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C173">
+        <v>498</v>
+      </c>
+      <c r="D173">
+        <v>19</v>
+      </c>
+      <c r="E173">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C174">
+        <v>329</v>
+      </c>
+      <c r="D174">
+        <v>15</v>
+      </c>
+      <c r="E174">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C175">
+        <v>220</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C176">
+        <v>101</v>
+      </c>
+      <c r="D176">
+        <v>22</v>
+      </c>
+      <c r="E176">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C177">
+        <v>40</v>
+      </c>
+      <c r="D177">
+        <v>33</v>
+      </c>
+      <c r="E177">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C178">
+        <v>85</v>
+      </c>
+      <c r="D178">
+        <v>55</v>
+      </c>
+      <c r="E178">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12064,10 +12692,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14945,6 +15573,163 @@
         <v>9</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170">
+        <v>18</v>
+      </c>
+      <c r="D170">
+        <v>6</v>
+      </c>
+      <c r="E170">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C171">
+        <v>30</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172">
+        <v>52</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C173">
+        <v>38</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C174">
+        <v>51</v>
+      </c>
+      <c r="D174">
+        <v>3</v>
+      </c>
+      <c r="E174">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175">
+        <v>44</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176">
+        <v>9</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C177">
+        <v>8</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C178">
+        <v>16</v>
+      </c>
+      <c r="D178">
+        <v>3</v>
+      </c>
+      <c r="E178">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14952,10 +15737,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17833,6 +18618,163 @@
         <v>0</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C170">
+        <v>22</v>
+      </c>
+      <c r="D170">
+        <v>1</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>20</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C172">
+        <v>14</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C173">
+        <v>11</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
+        <v>7</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C176">
+        <v>3</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
+        <v>12</v>
+      </c>
+      <c r="D177">
+        <v>0</v>
+      </c>
+      <c r="E177">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178">
+        <v>3</v>
+      </c>
+      <c r="D178">
+        <v>2</v>
+      </c>
+      <c r="E178">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17840,10 +18782,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20721,6 +21663,163 @@
         <v>16</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170">
+        <v>112</v>
+      </c>
+      <c r="D170">
+        <v>6</v>
+      </c>
+      <c r="E170">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C171">
+        <v>194</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+      <c r="E171">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172">
+        <v>114</v>
+      </c>
+      <c r="D172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173">
+        <v>165</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174">
+        <v>55</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>0</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176">
+        <v>67</v>
+      </c>
+      <c r="D176">
+        <v>3</v>
+      </c>
+      <c r="E176">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C177">
+        <v>116</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178">
+        <v>105</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20728,10 +21827,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23609,6 +24708,163 @@
         <v>518</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C170">
+        <v>179</v>
+      </c>
+      <c r="D170">
+        <v>31</v>
+      </c>
+      <c r="E170">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C171">
+        <v>262</v>
+      </c>
+      <c r="D171">
+        <v>14</v>
+      </c>
+      <c r="E171">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C172">
+        <v>136</v>
+      </c>
+      <c r="D172">
+        <v>30</v>
+      </c>
+      <c r="E172">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C173">
+        <v>162</v>
+      </c>
+      <c r="D173">
+        <v>12</v>
+      </c>
+      <c r="E173">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C174">
+        <v>94</v>
+      </c>
+      <c r="D174">
+        <v>57</v>
+      </c>
+      <c r="E174">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C175">
+        <v>23</v>
+      </c>
+      <c r="D175">
+        <v>15</v>
+      </c>
+      <c r="E175">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C176">
+        <v>152</v>
+      </c>
+      <c r="D176">
+        <v>17</v>
+      </c>
+      <c r="E176">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C177">
+        <v>193</v>
+      </c>
+      <c r="D177">
+        <v>23</v>
+      </c>
+      <c r="E177">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C178">
+        <v>154</v>
+      </c>
+      <c r="D178">
+        <v>22</v>
+      </c>
+      <c r="E178">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23616,10 +24872,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView topLeftCell="A159" workbookViewId="0">
+      <selection activeCell="B179" sqref="A179:B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26500,6 +27756,163 @@
         <v>22</v>
       </c>
     </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="14">
+        <v>44068</v>
+      </c>
+      <c r="B170" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170">
+        <v>84</v>
+      </c>
+      <c r="D170">
+        <v>4</v>
+      </c>
+      <c r="E170">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="14">
+        <v>44069</v>
+      </c>
+      <c r="B171" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C171">
+        <v>97</v>
+      </c>
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="14">
+        <v>44070</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172">
+        <v>148</v>
+      </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
+      <c r="E172">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="14">
+        <v>44071</v>
+      </c>
+      <c r="B173" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C173">
+        <v>199</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="14">
+        <v>44072</v>
+      </c>
+      <c r="B174" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C174">
+        <v>231</v>
+      </c>
+      <c r="D174">
+        <v>4</v>
+      </c>
+      <c r="E174">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="14">
+        <v>44073</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C175">
+        <v>274</v>
+      </c>
+      <c r="D175">
+        <v>4</v>
+      </c>
+      <c r="E175">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="14">
+        <v>44074</v>
+      </c>
+      <c r="B176" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176">
+        <v>120</v>
+      </c>
+      <c r="D176">
+        <v>3</v>
+      </c>
+      <c r="E176">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="14">
+        <v>44075</v>
+      </c>
+      <c r="B177" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C177">
+        <v>134</v>
+      </c>
+      <c r="D177">
+        <v>3</v>
+      </c>
+      <c r="E177">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="14">
+        <v>44076</v>
+      </c>
+      <c r="B178" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178">
+        <v>117</v>
+      </c>
+      <c r="D178">
+        <v>8</v>
+      </c>
+      <c r="E178">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
+      <c r="B179" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 6 de septiembre 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AB8918-0F80-41CD-9234-920D8474E1EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA403033-42BB-424F-BC54-E750F70E1AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="45" windowWidth="23325" windowHeight="11475" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="2445" yWindow="45" windowWidth="23325" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1638" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,8 +3547,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="4"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="4">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C179">
+        <v>82</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="4">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C180">
+        <v>18</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="4">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181">
+        <v>14</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="4">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>7</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3557,10 +3621,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E183"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C184" sqref="C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6592,8 +6656,77 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C179">
+        <v>43</v>
+      </c>
+      <c r="D179">
+        <v>8</v>
+      </c>
+      <c r="E179" s="10">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C180">
+        <v>30</v>
+      </c>
+      <c r="D180">
+        <v>5</v>
+      </c>
+      <c r="E180" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C181">
+        <v>26</v>
+      </c>
+      <c r="D181">
+        <v>7</v>
+      </c>
+      <c r="E181" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C182">
+        <v>9</v>
+      </c>
+      <c r="D182">
+        <v>5</v>
+      </c>
+      <c r="E182" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14"/>
+      <c r="B183" s="8"/>
+      <c r="E183" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6602,10 +6735,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9637,8 +9770,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="14"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>73</v>
+      </c>
+      <c r="D179">
+        <v>4</v>
+      </c>
+      <c r="E179">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180">
+        <v>63</v>
+      </c>
+      <c r="D180">
+        <v>7</v>
+      </c>
+      <c r="E180">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181">
+        <v>50</v>
+      </c>
+      <c r="D181">
+        <v>6</v>
+      </c>
+      <c r="E181">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C182">
+        <v>60</v>
+      </c>
+      <c r="D182">
+        <v>2</v>
+      </c>
+      <c r="E182">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9647,10 +9844,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12682,8 +12879,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C179">
+        <v>108</v>
+      </c>
+      <c r="D179">
+        <v>55</v>
+      </c>
+      <c r="E179">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C180">
+        <v>214</v>
+      </c>
+      <c r="D180">
+        <v>11</v>
+      </c>
+      <c r="E180">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C181">
+        <v>279</v>
+      </c>
+      <c r="D181">
+        <v>18</v>
+      </c>
+      <c r="E181">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C182">
+        <v>164</v>
+      </c>
+      <c r="D182">
+        <v>6</v>
+      </c>
+      <c r="E182">
+        <v>1219</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12692,10 +12953,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
     <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B180"/>
+      <selection activeCell="E183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15727,8 +15988,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="10"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179">
+        <v>102</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180">
+        <v>43</v>
+      </c>
+      <c r="D180">
+        <v>2</v>
+      </c>
+      <c r="E180">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C181">
+        <v>19</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182">
+        <v>28</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15737,10 +16062,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B180"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="E183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18772,8 +19097,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
+        <v>5</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180">
+        <v>7</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181">
+        <v>3</v>
+      </c>
+      <c r="D181">
+        <v>3</v>
+      </c>
+      <c r="E181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182">
+        <v>3</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18782,10 +19171,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21817,8 +22206,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C179">
+        <v>101</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180">
+        <v>178</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C181">
+        <v>68</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C182">
+        <v>108</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21827,10 +22280,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="C183" sqref="C183:E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24862,8 +25315,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C179">
+        <v>93</v>
+      </c>
+      <c r="D179">
+        <v>14</v>
+      </c>
+      <c r="E179">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C180">
+        <v>122</v>
+      </c>
+      <c r="D180">
+        <v>25</v>
+      </c>
+      <c r="E180">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C181">
+        <v>78</v>
+      </c>
+      <c r="D181">
+        <v>19</v>
+      </c>
+      <c r="E181">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182">
+        <v>27</v>
+      </c>
+      <c r="D182">
+        <v>1593</v>
+      </c>
+      <c r="E182">
+        <v>347</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24872,10 +25389,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E179"/>
+  <dimension ref="A1:E182"/>
   <sheetViews>
-    <sheetView topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="B179" sqref="A179:B179"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27910,8 +28427,72 @@
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="14"/>
-      <c r="B179" s="8"/>
+      <c r="A179" s="14">
+        <v>44077</v>
+      </c>
+      <c r="B179" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179">
+        <v>246</v>
+      </c>
+      <c r="D179">
+        <v>2</v>
+      </c>
+      <c r="E179">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="14">
+        <v>44078</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180">
+        <v>124</v>
+      </c>
+      <c r="D180">
+        <v>3</v>
+      </c>
+      <c r="E180">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="14">
+        <v>44079</v>
+      </c>
+      <c r="B181" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181">
+        <v>124</v>
+      </c>
+      <c r="D181">
+        <v>2</v>
+      </c>
+      <c r="E181">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="14">
+        <v>44080</v>
+      </c>
+      <c r="B182" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C182">
+        <v>122</v>
+      </c>
+      <c r="D182">
+        <v>4</v>
+      </c>
+      <c r="E182">
+        <v>149</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Actualizado hasta 20 de septiembre de 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA403033-42BB-424F-BC54-E750F70E1AC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8269002F-62E8-404B-A45C-F0EA1138802B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="45" windowWidth="23325" windowHeight="11475" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="26160" windowHeight="11760" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1674" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3614,6 +3614,227 @@
         <v>0</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="4">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C183">
+        <v>29</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+      <c r="E183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="4">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C184">
+        <v>25</v>
+      </c>
+      <c r="D184">
+        <v>2</v>
+      </c>
+      <c r="E184">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="4">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C185">
+        <v>27</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="4">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C186">
+        <v>40</v>
+      </c>
+      <c r="D186">
+        <v>2</v>
+      </c>
+      <c r="E186">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C187">
+        <v>20</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="4">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C188">
+        <v>4</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="4">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C189">
+        <v>17</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="4">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190">
+        <v>14</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+      <c r="E190">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="4">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="4">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C192">
+        <v>14</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="4">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C193">
+        <v>24</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="4">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C194">
+        <v>10</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="4">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C195">
+        <v>5</v>
+      </c>
+      <c r="D195">
+        <v>2</v>
+      </c>
+      <c r="E195">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3621,10 +3842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E183"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C184" sqref="C184"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6724,9 +6945,225 @@
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
-      <c r="B183" s="8"/>
-      <c r="E183" s="10"/>
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C183">
+        <v>5</v>
+      </c>
+      <c r="D183">
+        <v>7</v>
+      </c>
+      <c r="E183" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184">
+        <v>42</v>
+      </c>
+      <c r="D184">
+        <v>5</v>
+      </c>
+      <c r="E184" s="10">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C185">
+        <v>50</v>
+      </c>
+      <c r="D185">
+        <v>8</v>
+      </c>
+      <c r="E185" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C186">
+        <v>45</v>
+      </c>
+      <c r="D186">
+        <v>7</v>
+      </c>
+      <c r="E186" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C187">
+        <v>123</v>
+      </c>
+      <c r="D187">
+        <v>7</v>
+      </c>
+      <c r="E187" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C188">
+        <v>176</v>
+      </c>
+      <c r="D188">
+        <v>10</v>
+      </c>
+      <c r="E188" s="10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C189">
+        <v>77</v>
+      </c>
+      <c r="D189">
+        <v>6</v>
+      </c>
+      <c r="E189" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C190">
+        <v>50</v>
+      </c>
+      <c r="D190">
+        <v>5</v>
+      </c>
+      <c r="E190" s="10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C191">
+        <v>69</v>
+      </c>
+      <c r="D191">
+        <v>8</v>
+      </c>
+      <c r="E191" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C192">
+        <v>33</v>
+      </c>
+      <c r="D192">
+        <v>5</v>
+      </c>
+      <c r="E192" s="10">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C193">
+        <v>34</v>
+      </c>
+      <c r="D193">
+        <v>7</v>
+      </c>
+      <c r="E193" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C194">
+        <v>50</v>
+      </c>
+      <c r="D194">
+        <v>6</v>
+      </c>
+      <c r="E194" s="10">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C195">
+        <v>14</v>
+      </c>
+      <c r="D195">
+        <v>5</v>
+      </c>
+      <c r="E195" s="10">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6735,10 +7172,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="C197" sqref="C197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9837,6 +10274,227 @@
         <v>46</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183">
+        <v>21</v>
+      </c>
+      <c r="D183">
+        <v>3</v>
+      </c>
+      <c r="E183">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C184">
+        <v>78</v>
+      </c>
+      <c r="D184">
+        <v>8</v>
+      </c>
+      <c r="E184">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185">
+        <v>135</v>
+      </c>
+      <c r="D185">
+        <v>3</v>
+      </c>
+      <c r="E185">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C186">
+        <v>71</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C187">
+        <v>108</v>
+      </c>
+      <c r="D187">
+        <v>6</v>
+      </c>
+      <c r="E187">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C188">
+        <v>108</v>
+      </c>
+      <c r="D188">
+        <v>5</v>
+      </c>
+      <c r="E188">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189">
+        <v>77</v>
+      </c>
+      <c r="D189">
+        <v>3</v>
+      </c>
+      <c r="E189">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C190">
+        <v>64</v>
+      </c>
+      <c r="D190">
+        <v>4</v>
+      </c>
+      <c r="E190">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191">
+        <v>71</v>
+      </c>
+      <c r="D191">
+        <v>3</v>
+      </c>
+      <c r="E191">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C192">
+        <v>79</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C193">
+        <v>100</v>
+      </c>
+      <c r="D193">
+        <v>3</v>
+      </c>
+      <c r="E193">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C194">
+        <v>87</v>
+      </c>
+      <c r="D194">
+        <v>3</v>
+      </c>
+      <c r="E194">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195">
+        <v>34</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9844,10 +10502,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="E183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12946,6 +13604,227 @@
         <v>1219</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C183">
+        <v>272</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184">
+        <v>107</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C185">
+        <v>297</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C186">
+        <v>232</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C187">
+        <v>153</v>
+      </c>
+      <c r="D187">
+        <v>10</v>
+      </c>
+      <c r="E187">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C188">
+        <v>132</v>
+      </c>
+      <c r="D188">
+        <v>10</v>
+      </c>
+      <c r="E188">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C189">
+        <v>214</v>
+      </c>
+      <c r="D189">
+        <v>11</v>
+      </c>
+      <c r="E189">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C190">
+        <v>323</v>
+      </c>
+      <c r="D190">
+        <v>8</v>
+      </c>
+      <c r="E190">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C191">
+        <v>112</v>
+      </c>
+      <c r="D191">
+        <v>9</v>
+      </c>
+      <c r="E191">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C192">
+        <v>73</v>
+      </c>
+      <c r="D192">
+        <v>10</v>
+      </c>
+      <c r="E192">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C193">
+        <v>38</v>
+      </c>
+      <c r="D193">
+        <v>8</v>
+      </c>
+      <c r="E193">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C194">
+        <v>33</v>
+      </c>
+      <c r="D194">
+        <v>4</v>
+      </c>
+      <c r="E194">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C195">
+        <v>94</v>
+      </c>
+      <c r="D195">
+        <v>6</v>
+      </c>
+      <c r="E195">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12953,10 +13832,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="E183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16055,6 +16934,227 @@
         <v>9</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183">
+        <v>9</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>14</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C185">
+        <v>99</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186">
+        <v>51</v>
+      </c>
+      <c r="D186">
+        <v>5</v>
+      </c>
+      <c r="E186">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187">
+        <v>10</v>
+      </c>
+      <c r="D187">
+        <v>6</v>
+      </c>
+      <c r="E187">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188">
+        <v>21</v>
+      </c>
+      <c r="D188">
+        <v>0</v>
+      </c>
+      <c r="E188">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C189">
+        <v>33</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C190">
+        <v>29</v>
+      </c>
+      <c r="D190">
+        <v>5</v>
+      </c>
+      <c r="E190">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C191">
+        <v>9</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C192">
+        <v>25</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C193">
+        <v>17</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194">
+        <v>22</v>
+      </c>
+      <c r="D194">
+        <v>2</v>
+      </c>
+      <c r="E194">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C195">
+        <v>12</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16062,10 +17162,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="E183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="E194" sqref="E194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19164,6 +20264,227 @@
         <v>0</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+      <c r="E183">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C184">
+        <v>2</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>4</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>0</v>
+      </c>
+      <c r="E187">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>0</v>
+      </c>
+      <c r="E190">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C192">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>2</v>
+      </c>
+      <c r="E192">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+      <c r="D194">
+        <v>0</v>
+      </c>
+      <c r="E194">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19171,10 +20492,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22273,6 +23594,227 @@
         <v>53</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C183">
+        <v>174</v>
+      </c>
+      <c r="D183">
+        <v>6</v>
+      </c>
+      <c r="E183">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C184">
+        <v>172</v>
+      </c>
+      <c r="D184">
+        <v>4</v>
+      </c>
+      <c r="E184">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C185">
+        <v>183</v>
+      </c>
+      <c r="D185">
+        <v>7</v>
+      </c>
+      <c r="E185">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186">
+        <v>189</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C187">
+        <v>233</v>
+      </c>
+      <c r="D187">
+        <v>2</v>
+      </c>
+      <c r="E187">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188">
+        <v>89</v>
+      </c>
+      <c r="D188">
+        <v>2</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C189">
+        <v>39</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190">
+        <v>94</v>
+      </c>
+      <c r="D190">
+        <v>2</v>
+      </c>
+      <c r="E190">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C191">
+        <v>82</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+      <c r="E191">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192">
+        <v>50</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C193">
+        <v>21</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+      <c r="E193">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C194">
+        <v>112</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C195">
+        <v>13</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22280,10 +23822,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183:E185"/>
+    <sheetView topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25382,6 +26924,227 @@
         <v>347</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C183">
+        <v>85</v>
+      </c>
+      <c r="D183">
+        <v>19</v>
+      </c>
+      <c r="E183">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C184">
+        <v>117</v>
+      </c>
+      <c r="D184">
+        <v>20</v>
+      </c>
+      <c r="E184">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C185">
+        <v>116</v>
+      </c>
+      <c r="D185">
+        <v>25</v>
+      </c>
+      <c r="E185">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C186">
+        <v>125</v>
+      </c>
+      <c r="D186">
+        <v>27</v>
+      </c>
+      <c r="E186">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C187">
+        <v>98</v>
+      </c>
+      <c r="D187">
+        <v>21</v>
+      </c>
+      <c r="E187">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C188">
+        <v>38</v>
+      </c>
+      <c r="D188">
+        <v>18</v>
+      </c>
+      <c r="E188">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C189">
+        <v>68</v>
+      </c>
+      <c r="D189">
+        <v>22</v>
+      </c>
+      <c r="E189">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C190">
+        <v>60</v>
+      </c>
+      <c r="D190">
+        <v>30</v>
+      </c>
+      <c r="E190">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C191">
+        <v>104</v>
+      </c>
+      <c r="D191">
+        <v>26</v>
+      </c>
+      <c r="E191">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C192">
+        <v>68</v>
+      </c>
+      <c r="D192">
+        <v>8</v>
+      </c>
+      <c r="E192">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C193">
+        <v>73</v>
+      </c>
+      <c r="D193">
+        <v>12</v>
+      </c>
+      <c r="E193">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194">
+        <v>36</v>
+      </c>
+      <c r="D194">
+        <v>10</v>
+      </c>
+      <c r="E194">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C195">
+        <v>53</v>
+      </c>
+      <c r="D195">
+        <v>19</v>
+      </c>
+      <c r="E195">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25389,10 +27152,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E182"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
-      <selection activeCell="F169" sqref="F169"/>
+    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
+      <selection activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28494,6 +30257,227 @@
         <v>149</v>
       </c>
     </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="14">
+        <v>44081</v>
+      </c>
+      <c r="B183" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C183">
+        <v>238</v>
+      </c>
+      <c r="D183">
+        <v>7</v>
+      </c>
+      <c r="E183">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="14">
+        <v>44082</v>
+      </c>
+      <c r="B184" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184">
+        <v>147</v>
+      </c>
+      <c r="D184">
+        <v>4</v>
+      </c>
+      <c r="E184">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="14">
+        <v>44083</v>
+      </c>
+      <c r="B185" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>129</v>
+      </c>
+      <c r="D185">
+        <v>5</v>
+      </c>
+      <c r="E185">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="14">
+        <v>44084</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C186">
+        <v>107</v>
+      </c>
+      <c r="D186">
+        <v>2</v>
+      </c>
+      <c r="E186">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="14">
+        <v>44085</v>
+      </c>
+      <c r="B187" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C187">
+        <v>222</v>
+      </c>
+      <c r="D187">
+        <v>5</v>
+      </c>
+      <c r="E187">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="14">
+        <v>44086</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C188">
+        <v>242</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+      <c r="E188">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="14">
+        <v>44087</v>
+      </c>
+      <c r="B189" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C189">
+        <v>284</v>
+      </c>
+      <c r="D189">
+        <v>5</v>
+      </c>
+      <c r="E189">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="14">
+        <v>44088</v>
+      </c>
+      <c r="B190" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C190">
+        <v>195</v>
+      </c>
+      <c r="D190">
+        <v>4</v>
+      </c>
+      <c r="E190">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="14">
+        <v>44089</v>
+      </c>
+      <c r="B191" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C191">
+        <v>219</v>
+      </c>
+      <c r="D191">
+        <v>3</v>
+      </c>
+      <c r="E191">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="14">
+        <v>44090</v>
+      </c>
+      <c r="B192" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C192">
+        <v>242</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="14">
+        <v>44091</v>
+      </c>
+      <c r="B193" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C193">
+        <v>240</v>
+      </c>
+      <c r="D193">
+        <v>3</v>
+      </c>
+      <c r="E193">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="14">
+        <v>44092</v>
+      </c>
+      <c r="B194" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C194">
+        <v>280</v>
+      </c>
+      <c r="D194">
+        <v>3</v>
+      </c>
+      <c r="E194">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="14">
+        <v>44093</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C195">
+        <v>194</v>
+      </c>
+      <c r="D195">
+        <v>4</v>
+      </c>
+      <c r="E195">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado 8 de octubre 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8269002F-62E8-404B-A45C-F0EA1138802B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F318822-0AFC-4939-8D2A-A48C87A98FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="26160" windowHeight="11760" activeTab="8" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="1050" yWindow="0" windowWidth="12720" windowHeight="11265" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1791" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B215" sqref="B215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,6 +3835,329 @@
         <v>90</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="4">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="4">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C197">
+        <v>3</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="4">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C198">
+        <v>23</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="4">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C199">
+        <v>40</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+      <c r="E199">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="4">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C200">
+        <v>20</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+      <c r="E200">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="4">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <v>15</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="4">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <v>5</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="4">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C203">
+        <v>0</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="4">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+      <c r="D204">
+        <v>2</v>
+      </c>
+      <c r="E204">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="4">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+      <c r="D205">
+        <v>4</v>
+      </c>
+      <c r="E205">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="4">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C206">
+        <v>7</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+      <c r="E206">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="4">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C207">
+        <v>32</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="4">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C208">
+        <v>16</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+      <c r="E208">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="4">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C209">
+        <v>10</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="4">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="4">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C211">
+        <v>3</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="4">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="4">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="4">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C214">
+        <v>5</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3842,10 +4165,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7165,6 +7488,329 @@
         <v>95</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C196">
+        <v>2</v>
+      </c>
+      <c r="D196">
+        <v>4</v>
+      </c>
+      <c r="E196" s="10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C197">
+        <v>28</v>
+      </c>
+      <c r="D197">
+        <v>6</v>
+      </c>
+      <c r="E197" s="10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C198">
+        <v>7</v>
+      </c>
+      <c r="D198">
+        <v>5</v>
+      </c>
+      <c r="E198" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C199">
+        <v>22</v>
+      </c>
+      <c r="D199">
+        <v>6</v>
+      </c>
+      <c r="E199" s="10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C200">
+        <v>37</v>
+      </c>
+      <c r="D200">
+        <v>5</v>
+      </c>
+      <c r="E200" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C201">
+        <v>19</v>
+      </c>
+      <c r="D201">
+        <v>7</v>
+      </c>
+      <c r="E201" s="10">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C202">
+        <v>22</v>
+      </c>
+      <c r="D202">
+        <v>6</v>
+      </c>
+      <c r="E202" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C203">
+        <v>4</v>
+      </c>
+      <c r="D203">
+        <v>4</v>
+      </c>
+      <c r="E203" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C204">
+        <v>30</v>
+      </c>
+      <c r="D204">
+        <v>7</v>
+      </c>
+      <c r="E204" s="10">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C205">
+        <v>31</v>
+      </c>
+      <c r="D205">
+        <v>5</v>
+      </c>
+      <c r="E205" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C206">
+        <v>17</v>
+      </c>
+      <c r="D206">
+        <v>6</v>
+      </c>
+      <c r="E206" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C207">
+        <v>15</v>
+      </c>
+      <c r="D207">
+        <v>6</v>
+      </c>
+      <c r="E207" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C208">
+        <v>18</v>
+      </c>
+      <c r="D208">
+        <v>7</v>
+      </c>
+      <c r="E208" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+      <c r="D209">
+        <v>5</v>
+      </c>
+      <c r="E209" s="10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C210">
+        <v>12</v>
+      </c>
+      <c r="D210">
+        <v>7</v>
+      </c>
+      <c r="E210" s="10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C211">
+        <v>14</v>
+      </c>
+      <c r="D211">
+        <v>5</v>
+      </c>
+      <c r="E211" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C212">
+        <v>33</v>
+      </c>
+      <c r="D212">
+        <v>5</v>
+      </c>
+      <c r="E212" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C213">
+        <v>22</v>
+      </c>
+      <c r="D213">
+        <v>6</v>
+      </c>
+      <c r="E213" s="10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C214">
+        <v>7</v>
+      </c>
+      <c r="D214">
+        <v>6</v>
+      </c>
+      <c r="E214" s="10">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7172,10 +7818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="C197" sqref="C197"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10495,6 +11141,329 @@
         <v>45</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C196">
+        <v>41</v>
+      </c>
+      <c r="D196">
+        <v>3</v>
+      </c>
+      <c r="E196">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197">
+        <v>16</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C198">
+        <v>73</v>
+      </c>
+      <c r="D198">
+        <v>2</v>
+      </c>
+      <c r="E198">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199">
+        <v>48</v>
+      </c>
+      <c r="D199">
+        <v>2</v>
+      </c>
+      <c r="E199">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C200">
+        <v>62</v>
+      </c>
+      <c r="D200">
+        <v>2</v>
+      </c>
+      <c r="E200">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201">
+        <v>61</v>
+      </c>
+      <c r="D201">
+        <v>2</v>
+      </c>
+      <c r="E201">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202">
+        <v>46</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203">
+        <v>46</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204">
+        <v>23</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+      <c r="E204">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <v>14</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+      <c r="E205">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C206">
+        <v>31</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207">
+        <v>28</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C208">
+        <v>25</v>
+      </c>
+      <c r="D208">
+        <v>3</v>
+      </c>
+      <c r="E208">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209">
+        <v>34</v>
+      </c>
+      <c r="D209">
+        <v>3</v>
+      </c>
+      <c r="E209">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C210">
+        <v>24</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211">
+        <v>18</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C212">
+        <v>14</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213">
+        <v>14</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C214">
+        <v>59</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10502,10 +11471,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13825,6 +14794,329 @@
         <v>49</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C196">
+        <v>34</v>
+      </c>
+      <c r="D196">
+        <v>4</v>
+      </c>
+      <c r="E196">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C197">
+        <v>27</v>
+      </c>
+      <c r="D197">
+        <v>4</v>
+      </c>
+      <c r="E197">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C198">
+        <v>37</v>
+      </c>
+      <c r="D198">
+        <v>4</v>
+      </c>
+      <c r="E198">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C199">
+        <v>24</v>
+      </c>
+      <c r="D199">
+        <v>4</v>
+      </c>
+      <c r="E199">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C200">
+        <v>45</v>
+      </c>
+      <c r="D200">
+        <v>5</v>
+      </c>
+      <c r="E200">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C201">
+        <v>45</v>
+      </c>
+      <c r="D201">
+        <v>5</v>
+      </c>
+      <c r="E201">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C202">
+        <v>52</v>
+      </c>
+      <c r="D202">
+        <v>4</v>
+      </c>
+      <c r="E202">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C203">
+        <v>29</v>
+      </c>
+      <c r="D203">
+        <v>4</v>
+      </c>
+      <c r="E203">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C204">
+        <v>17</v>
+      </c>
+      <c r="D204">
+        <v>3</v>
+      </c>
+      <c r="E204">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+      <c r="E205">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C206">
+        <v>29</v>
+      </c>
+      <c r="D206">
+        <v>6</v>
+      </c>
+      <c r="E206">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C207">
+        <v>40</v>
+      </c>
+      <c r="D207">
+        <v>7</v>
+      </c>
+      <c r="E207">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C208">
+        <v>40</v>
+      </c>
+      <c r="D208">
+        <v>7</v>
+      </c>
+      <c r="E208">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C209">
+        <v>28</v>
+      </c>
+      <c r="D209">
+        <v>5</v>
+      </c>
+      <c r="E209">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C210">
+        <v>14</v>
+      </c>
+      <c r="D210">
+        <v>3</v>
+      </c>
+      <c r="E210">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C211">
+        <v>16</v>
+      </c>
+      <c r="D211">
+        <v>3</v>
+      </c>
+      <c r="E211">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C213">
+        <v>49</v>
+      </c>
+      <c r="D213">
+        <v>9</v>
+      </c>
+      <c r="E213">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C214">
+        <v>22</v>
+      </c>
+      <c r="D214">
+        <v>6</v>
+      </c>
+      <c r="E214">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13832,10 +15124,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A188" workbookViewId="0">
-      <selection activeCell="D194" sqref="D194"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17155,6 +18447,329 @@
         <v>54</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196">
+        <v>22</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C197">
+        <v>6</v>
+      </c>
+      <c r="D197">
+        <v>2</v>
+      </c>
+      <c r="E197">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198">
+        <v>10</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C199">
+        <v>41</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200">
+        <v>44</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C201">
+        <v>29</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+      <c r="E201">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C203">
+        <v>18</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C204">
+        <v>14</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C205">
+        <v>8</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C206">
+        <v>12</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C207">
+        <v>13</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C208">
+        <v>18</v>
+      </c>
+      <c r="D208">
+        <v>4</v>
+      </c>
+      <c r="E208">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C209">
+        <v>10</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C210">
+        <v>13</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C211">
+        <v>2</v>
+      </c>
+      <c r="D211">
+        <v>2</v>
+      </c>
+      <c r="E211">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C212">
+        <v>11</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C213">
+        <v>13</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C214">
+        <v>10</v>
+      </c>
+      <c r="D214">
+        <v>3</v>
+      </c>
+      <c r="E214">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17162,10 +18777,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView topLeftCell="A182" workbookViewId="0">
-      <selection activeCell="E194" sqref="E194"/>
+    <sheetView topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="C216" sqref="C216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20485,6 +22100,337 @@
         <v>0</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+      <c r="E198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199">
+        <v>0</v>
+      </c>
+      <c r="E199">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+      <c r="E200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C202">
+        <v>0</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <v>0</v>
+      </c>
+      <c r="E203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+      <c r="E204">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+      <c r="D208">
+        <v>0</v>
+      </c>
+      <c r="E208">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C209">
+        <v>0</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+      <c r="D211">
+        <v>0</v>
+      </c>
+      <c r="E211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14"/>
+      <c r="B215" s="8"/>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14"/>
+      <c r="B216" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20492,10 +22438,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="E190" sqref="E190"/>
+    <sheetView topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="E215" sqref="D215:E218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23815,6 +25761,329 @@
         <v>18</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196">
+        <v>16</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+      <c r="E196">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C197">
+        <v>54</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+      <c r="E197">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C198">
+        <v>54</v>
+      </c>
+      <c r="D198">
+        <v>6</v>
+      </c>
+      <c r="E198">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C199">
+        <v>135</v>
+      </c>
+      <c r="D199">
+        <v>5</v>
+      </c>
+      <c r="E199">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C200">
+        <v>63</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+      <c r="E200">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201">
+        <v>67</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C202">
+        <v>82</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+      <c r="E202">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203">
+        <v>11</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+      <c r="E203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204">
+        <v>40</v>
+      </c>
+      <c r="D204">
+        <v>5</v>
+      </c>
+      <c r="E204">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205">
+        <v>40</v>
+      </c>
+      <c r="D205">
+        <v>0</v>
+      </c>
+      <c r="E205">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C206">
+        <v>70</v>
+      </c>
+      <c r="D206">
+        <v>0</v>
+      </c>
+      <c r="E206">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C207">
+        <v>24</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+      <c r="E207">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C208">
+        <v>67</v>
+      </c>
+      <c r="D208">
+        <v>2</v>
+      </c>
+      <c r="E208">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C209">
+        <v>75</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C210">
+        <v>55</v>
+      </c>
+      <c r="D210">
+        <v>1</v>
+      </c>
+      <c r="E210">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C211">
+        <v>25</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+      <c r="E211">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C212">
+        <v>56</v>
+      </c>
+      <c r="D212">
+        <v>0</v>
+      </c>
+      <c r="E212">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213">
+        <v>41</v>
+      </c>
+      <c r="D213">
+        <v>2</v>
+      </c>
+      <c r="E213">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214">
+        <v>35</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23822,10 +26091,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="E217" sqref="E215:E217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27145,6 +29414,329 @@
         <v>115</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C196">
+        <v>25</v>
+      </c>
+      <c r="D196">
+        <v>16</v>
+      </c>
+      <c r="E196">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C197">
+        <v>48</v>
+      </c>
+      <c r="D197">
+        <v>18</v>
+      </c>
+      <c r="E197">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198">
+        <v>50</v>
+      </c>
+      <c r="D198">
+        <v>18</v>
+      </c>
+      <c r="E198">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C199">
+        <v>60</v>
+      </c>
+      <c r="D199">
+        <v>17</v>
+      </c>
+      <c r="E199">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C200">
+        <v>38</v>
+      </c>
+      <c r="D200">
+        <v>15</v>
+      </c>
+      <c r="E200">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C201">
+        <v>134</v>
+      </c>
+      <c r="D201">
+        <v>17</v>
+      </c>
+      <c r="E201">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202">
+        <v>36</v>
+      </c>
+      <c r="D202">
+        <v>17</v>
+      </c>
+      <c r="E202">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C203">
+        <v>44</v>
+      </c>
+      <c r="D203">
+        <v>18</v>
+      </c>
+      <c r="E203">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C204">
+        <v>37</v>
+      </c>
+      <c r="D204">
+        <v>15</v>
+      </c>
+      <c r="E204">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C205">
+        <v>59</v>
+      </c>
+      <c r="D205">
+        <v>17</v>
+      </c>
+      <c r="E205">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206">
+        <v>37</v>
+      </c>
+      <c r="D206">
+        <v>16</v>
+      </c>
+      <c r="E206">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C207">
+        <v>25</v>
+      </c>
+      <c r="D207">
+        <v>13</v>
+      </c>
+      <c r="E207">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C208">
+        <v>101</v>
+      </c>
+      <c r="D208">
+        <v>17</v>
+      </c>
+      <c r="E208">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C209">
+        <v>37</v>
+      </c>
+      <c r="D209">
+        <v>13</v>
+      </c>
+      <c r="E209">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C210">
+        <v>43</v>
+      </c>
+      <c r="D210">
+        <v>16</v>
+      </c>
+      <c r="E210">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C211">
+        <v>26</v>
+      </c>
+      <c r="D211">
+        <v>13</v>
+      </c>
+      <c r="E211">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C212">
+        <v>69</v>
+      </c>
+      <c r="D212">
+        <v>15</v>
+      </c>
+      <c r="E212">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C213">
+        <v>53</v>
+      </c>
+      <c r="D213">
+        <v>15</v>
+      </c>
+      <c r="E213">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214">
+        <v>47</v>
+      </c>
+      <c r="D214">
+        <v>17</v>
+      </c>
+      <c r="E214">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27152,10 +29744,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" workbookViewId="0">
-      <selection activeCell="D197" sqref="D197"/>
+    <sheetView topLeftCell="A195" workbookViewId="0">
+      <selection activeCell="E215" sqref="D215:E217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30478,6 +33070,329 @@
         <v>109</v>
       </c>
     </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="14">
+        <v>44094</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C196">
+        <v>65</v>
+      </c>
+      <c r="D196">
+        <v>3</v>
+      </c>
+      <c r="E196">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="14">
+        <v>44095</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C197">
+        <v>128</v>
+      </c>
+      <c r="D197">
+        <v>6</v>
+      </c>
+      <c r="E197">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="14">
+        <v>44096</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C198">
+        <v>212</v>
+      </c>
+      <c r="D198">
+        <v>3</v>
+      </c>
+      <c r="E198">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="14">
+        <v>44097</v>
+      </c>
+      <c r="B199" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C199">
+        <v>167</v>
+      </c>
+      <c r="D199">
+        <v>3</v>
+      </c>
+      <c r="E199">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="14">
+        <v>44098</v>
+      </c>
+      <c r="B200" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C200">
+        <v>318</v>
+      </c>
+      <c r="D200">
+        <v>5</v>
+      </c>
+      <c r="E200">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="14">
+        <v>44099</v>
+      </c>
+      <c r="B201" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C201">
+        <v>234</v>
+      </c>
+      <c r="D201">
+        <v>3</v>
+      </c>
+      <c r="E201">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="14">
+        <v>44100</v>
+      </c>
+      <c r="B202" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C202">
+        <v>127</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+      <c r="E202">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="14">
+        <v>44101</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C203">
+        <v>156</v>
+      </c>
+      <c r="D203">
+        <v>3</v>
+      </c>
+      <c r="E203">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="14">
+        <v>44102</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C204">
+        <v>160</v>
+      </c>
+      <c r="D204">
+        <v>8</v>
+      </c>
+      <c r="E204">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="14">
+        <v>44103</v>
+      </c>
+      <c r="B205" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C205">
+        <v>262</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+      <c r="E205">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="14">
+        <v>44104</v>
+      </c>
+      <c r="B206" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C206">
+        <v>466</v>
+      </c>
+      <c r="D206">
+        <v>5</v>
+      </c>
+      <c r="E206">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="14">
+        <v>44105</v>
+      </c>
+      <c r="B207" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C207">
+        <v>227</v>
+      </c>
+      <c r="D207">
+        <v>7</v>
+      </c>
+      <c r="E207">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="14">
+        <v>44106</v>
+      </c>
+      <c r="B208" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C208">
+        <v>218</v>
+      </c>
+      <c r="D208">
+        <v>3</v>
+      </c>
+      <c r="E208">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="14">
+        <v>44107</v>
+      </c>
+      <c r="B209" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209">
+        <v>153</v>
+      </c>
+      <c r="D209">
+        <v>2</v>
+      </c>
+      <c r="E209">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="14">
+        <v>44108</v>
+      </c>
+      <c r="B210" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210">
+        <v>138</v>
+      </c>
+      <c r="D210">
+        <v>1</v>
+      </c>
+      <c r="E210">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="14">
+        <v>44109</v>
+      </c>
+      <c r="B211" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211">
+        <v>135</v>
+      </c>
+      <c r="D211">
+        <v>2</v>
+      </c>
+      <c r="E211">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="14">
+        <v>44110</v>
+      </c>
+      <c r="B212" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <v>177</v>
+      </c>
+      <c r="D212">
+        <v>5</v>
+      </c>
+      <c r="E212">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="14">
+        <v>44111</v>
+      </c>
+      <c r="B213" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213">
+        <v>46</v>
+      </c>
+      <c r="D213">
+        <v>4</v>
+      </c>
+      <c r="E213">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="14">
+        <v>44112</v>
+      </c>
+      <c r="B214" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C214">
+        <v>78</v>
+      </c>
+      <c r="D214">
+        <v>2</v>
+      </c>
+      <c r="E214">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado hasta el 8 de noviembre del 2020
</commit_message>
<xml_diff>
--- a/BD/BD_dpto.xlsx
+++ b/BD/BD_dpto.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bladimir\Documents\Proyectos\COVID-19 Bolivia\COVID-19-Bolivia\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F318822-0AFC-4939-8D2A-A48C87A98FDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A9A428-A1C8-43DD-BD18-3D48AA3D82D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="0" windowWidth="12720" windowHeight="11265" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="26175" windowHeight="11760" xr2:uid="{3A21730E-5A1A-4345-88BB-DB068C0A42B3}"/>
   </bookViews>
   <sheets>
     <sheet name="bn" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">tj!$A$1:$E$133</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2241" uniqueCount="14">
   <si>
     <t>depto</t>
   </si>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -195,6 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F097565D-B4F2-4FAD-A8A5-BA14BCC36C69}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="B215" sqref="B215"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="C245" sqref="C245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4158,6 +4159,533 @@
         <v>60</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C215">
+        <v>13</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="4">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>18</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C217">
+        <v>7</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="4">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C219">
+        <v>4</v>
+      </c>
+      <c r="D219">
+        <v>1</v>
+      </c>
+      <c r="E219">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="4">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C221">
+        <v>2</v>
+      </c>
+      <c r="D221">
+        <v>0</v>
+      </c>
+      <c r="E221">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="4">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C222">
+        <v>17</v>
+      </c>
+      <c r="D222">
+        <v>1</v>
+      </c>
+      <c r="E222">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C223">
+        <v>2</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="4">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C225">
+        <v>1</v>
+      </c>
+      <c r="D225">
+        <v>1</v>
+      </c>
+      <c r="E225">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="4">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C226">
+        <v>8</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C227">
+        <v>4</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="4">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C228">
+        <v>4</v>
+      </c>
+      <c r="D228">
+        <v>1</v>
+      </c>
+      <c r="E228">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+      <c r="D229">
+        <v>1</v>
+      </c>
+      <c r="E229">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="4">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C230">
+        <v>3</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="4">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="4">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="4">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="4">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+      <c r="E238">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="4">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C240">
+        <v>6</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C241">
+        <v>5</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="4">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C242">
+        <v>5</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C243">
+        <v>6</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+      <c r="E243">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="4">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4165,10 +4693,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A4E8676-9862-491A-957F-B26AD53C440D}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E215" sqref="E215"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7811,6 +8339,533 @@
         <v>50</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C215">
+        <v>15</v>
+      </c>
+      <c r="D215">
+        <v>5</v>
+      </c>
+      <c r="E215" s="10">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C216">
+        <v>4</v>
+      </c>
+      <c r="D216">
+        <v>5</v>
+      </c>
+      <c r="E216" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217">
+        <v>3</v>
+      </c>
+      <c r="E217" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C218">
+        <v>11</v>
+      </c>
+      <c r="D218">
+        <v>4</v>
+      </c>
+      <c r="E218" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C219">
+        <v>19</v>
+      </c>
+      <c r="D219">
+        <v>5</v>
+      </c>
+      <c r="E219" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C220">
+        <v>3</v>
+      </c>
+      <c r="D220">
+        <v>3</v>
+      </c>
+      <c r="E220" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C221">
+        <v>23</v>
+      </c>
+      <c r="D221">
+        <v>5</v>
+      </c>
+      <c r="E221" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C222">
+        <v>17</v>
+      </c>
+      <c r="D222">
+        <v>5</v>
+      </c>
+      <c r="E222" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C223">
+        <v>6</v>
+      </c>
+      <c r="D223">
+        <v>4</v>
+      </c>
+      <c r="E223" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>3</v>
+      </c>
+      <c r="E224" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C225">
+        <v>24</v>
+      </c>
+      <c r="D225">
+        <v>5</v>
+      </c>
+      <c r="E225" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C226">
+        <v>15</v>
+      </c>
+      <c r="D226">
+        <v>4</v>
+      </c>
+      <c r="E226" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C227">
+        <v>23</v>
+      </c>
+      <c r="D227">
+        <v>5</v>
+      </c>
+      <c r="E227" s="10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C228">
+        <v>13</v>
+      </c>
+      <c r="D228">
+        <v>6</v>
+      </c>
+      <c r="E228" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+      <c r="D229">
+        <v>5</v>
+      </c>
+      <c r="E229" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C230">
+        <v>4</v>
+      </c>
+      <c r="D230">
+        <v>4</v>
+      </c>
+      <c r="E230" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+      <c r="D231">
+        <v>2</v>
+      </c>
+      <c r="E231" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C232">
+        <v>12</v>
+      </c>
+      <c r="D232">
+        <v>3</v>
+      </c>
+      <c r="E232" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C233">
+        <v>6</v>
+      </c>
+      <c r="D233">
+        <v>5</v>
+      </c>
+      <c r="E233" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C234">
+        <v>13</v>
+      </c>
+      <c r="D234">
+        <v>5</v>
+      </c>
+      <c r="E234" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C235">
+        <v>21</v>
+      </c>
+      <c r="D235">
+        <v>4</v>
+      </c>
+      <c r="E235" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C236">
+        <v>11</v>
+      </c>
+      <c r="D236">
+        <v>4</v>
+      </c>
+      <c r="E236" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>2</v>
+      </c>
+      <c r="E237" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C239">
+        <v>10</v>
+      </c>
+      <c r="D239">
+        <v>3</v>
+      </c>
+      <c r="E239" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240">
+        <v>3</v>
+      </c>
+      <c r="E240" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C241">
+        <v>11</v>
+      </c>
+      <c r="D241">
+        <v>5</v>
+      </c>
+      <c r="E241" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C242">
+        <v>12</v>
+      </c>
+      <c r="D242">
+        <v>3</v>
+      </c>
+      <c r="E242" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C243">
+        <v>3</v>
+      </c>
+      <c r="D243">
+        <v>5</v>
+      </c>
+      <c r="E243" s="10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C244">
+        <v>7</v>
+      </c>
+      <c r="D244">
+        <v>3</v>
+      </c>
+      <c r="E244" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C245">
+        <v>2</v>
+      </c>
+      <c r="D245">
+        <v>4</v>
+      </c>
+      <c r="E245" s="10">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7818,10 +8873,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04516DF9-9120-48B2-8BB4-0DE7888FEF36}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E215" sqref="E215"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11464,6 +12519,533 @@
         <v>63</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215">
+        <v>23</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C216">
+        <v>15</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217">
+        <v>8</v>
+      </c>
+      <c r="D217">
+        <v>2</v>
+      </c>
+      <c r="E217">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C218">
+        <v>20</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C219">
+        <v>32</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C220">
+        <v>19</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C221">
+        <v>11</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+      <c r="E221">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C222">
+        <v>32</v>
+      </c>
+      <c r="D222">
+        <v>3</v>
+      </c>
+      <c r="E222">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C223">
+        <v>43</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C224">
+        <v>20</v>
+      </c>
+      <c r="D224">
+        <v>1</v>
+      </c>
+      <c r="E224">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225">
+        <v>6</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C226">
+        <v>19</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C227">
+        <v>17</v>
+      </c>
+      <c r="D227">
+        <v>2</v>
+      </c>
+      <c r="E227">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C228">
+        <v>20</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C229">
+        <v>30</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C230">
+        <v>31</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C231">
+        <v>31</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C232">
+        <v>15</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C233">
+        <v>15</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C234">
+        <v>34</v>
+      </c>
+      <c r="D234">
+        <v>2</v>
+      </c>
+      <c r="E234">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C235">
+        <v>21</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C236">
+        <v>16</v>
+      </c>
+      <c r="D236">
+        <v>1</v>
+      </c>
+      <c r="E236">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C237">
+        <v>15</v>
+      </c>
+      <c r="D237">
+        <v>2</v>
+      </c>
+      <c r="E237">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C238">
+        <v>14</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C239">
+        <v>9</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C240">
+        <v>5</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C241">
+        <v>12</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C242">
+        <v>6</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="E242">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C243">
+        <v>14</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="E243">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C244">
+        <v>4</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C245">
+        <v>9</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11471,10 +13053,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2237256F-A74E-4670-8E7E-4A11CD5D023A}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E215" sqref="E215"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15117,6 +16699,533 @@
         <v>146</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215">
+        <v>47</v>
+      </c>
+      <c r="D215">
+        <v>7</v>
+      </c>
+      <c r="E215">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C216">
+        <v>30</v>
+      </c>
+      <c r="D216">
+        <v>8</v>
+      </c>
+      <c r="E216">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C217">
+        <v>8</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C218">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C219">
+        <v>19</v>
+      </c>
+      <c r="D219">
+        <v>5</v>
+      </c>
+      <c r="E219">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C220">
+        <v>12</v>
+      </c>
+      <c r="D220">
+        <v>5</v>
+      </c>
+      <c r="E220" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C221">
+        <v>36</v>
+      </c>
+      <c r="D221">
+        <v>7</v>
+      </c>
+      <c r="E221">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C222">
+        <v>27</v>
+      </c>
+      <c r="D222">
+        <v>5</v>
+      </c>
+      <c r="E222">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C223">
+        <v>11</v>
+      </c>
+      <c r="D223">
+        <v>3</v>
+      </c>
+      <c r="E223">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C224">
+        <v>9</v>
+      </c>
+      <c r="D224">
+        <v>2</v>
+      </c>
+      <c r="E224">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C225">
+        <v>6</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C226">
+        <v>9</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+      <c r="E226">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C227">
+        <v>30</v>
+      </c>
+      <c r="D227">
+        <v>4</v>
+      </c>
+      <c r="E227">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C228">
+        <v>11</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+      <c r="E228">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C229">
+        <v>19</v>
+      </c>
+      <c r="D229">
+        <v>3</v>
+      </c>
+      <c r="E229">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C230">
+        <v>29</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C231">
+        <v>13</v>
+      </c>
+      <c r="D231">
+        <v>2</v>
+      </c>
+      <c r="E231">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C232">
+        <v>2</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C233">
+        <v>29</v>
+      </c>
+      <c r="D233">
+        <v>4</v>
+      </c>
+      <c r="E233">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C234">
+        <v>29</v>
+      </c>
+      <c r="D234">
+        <v>4</v>
+      </c>
+      <c r="E234">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C235">
+        <v>18</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+      <c r="E235">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C236">
+        <v>46</v>
+      </c>
+      <c r="D236">
+        <v>2</v>
+      </c>
+      <c r="E236">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C237">
+        <v>15</v>
+      </c>
+      <c r="D237">
+        <v>1</v>
+      </c>
+      <c r="E237">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238">
+        <v>18</v>
+      </c>
+      <c r="D238">
+        <v>1</v>
+      </c>
+      <c r="E238">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+      <c r="E239">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C240">
+        <v>5</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+      <c r="E240">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C241">
+        <v>10</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+      <c r="E241">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C242">
+        <v>38</v>
+      </c>
+      <c r="D242">
+        <v>2</v>
+      </c>
+      <c r="E242">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C243">
+        <v>13</v>
+      </c>
+      <c r="D243">
+        <v>2</v>
+      </c>
+      <c r="E243">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C244">
+        <v>14</v>
+      </c>
+      <c r="D244">
+        <v>3</v>
+      </c>
+      <c r="E244">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C245">
+        <v>11</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>116</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15124,10 +17233,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B768E7FD-1810-4DC6-8633-BE7C9F0A3EE4}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="E215" sqref="E215"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18770,6 +20879,533 @@
         <v>67</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C215">
+        <v>23</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C216">
+        <v>13</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C217">
+        <v>12</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C218">
+        <v>8</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C219">
+        <v>11</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C220">
+        <v>8</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221">
+        <v>3</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C222">
+        <v>5</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C223">
+        <v>9</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C224">
+        <v>8</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C225">
+        <v>2</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C226">
+        <v>4</v>
+      </c>
+      <c r="D226">
+        <v>2</v>
+      </c>
+      <c r="E226">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C227">
+        <v>6</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C228">
+        <v>13</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C229">
+        <v>9</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C230">
+        <v>5</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C231">
+        <v>5</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+      <c r="D232">
+        <v>3</v>
+      </c>
+      <c r="E232">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C233">
+        <v>4</v>
+      </c>
+      <c r="D233">
+        <v>1</v>
+      </c>
+      <c r="E233">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C234">
+        <v>8</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+      <c r="E234">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C235">
+        <v>16</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C236">
+        <v>8</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C237">
+        <v>9</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C238">
+        <v>7</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+      <c r="D240">
+        <v>3</v>
+      </c>
+      <c r="E240">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C241">
+        <v>6</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C242">
+        <v>4</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="E242">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C243">
+        <v>11</v>
+      </c>
+      <c r="D243">
+        <v>2</v>
+      </c>
+      <c r="E243">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C244">
+        <v>2</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C245">
+        <v>16</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18777,10 +21413,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD8C9AB-E842-4AE9-BE28-6072ABCB926B}">
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22424,12 +25060,531 @@
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" s="14"/>
-      <c r="B215" s="8"/>
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>0</v>
+      </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
-      <c r="B216" s="8"/>
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216">
+        <v>0</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220">
+        <v>2</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221">
+        <v>0</v>
+      </c>
+      <c r="D221">
+        <v>0</v>
+      </c>
+      <c r="E221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C226">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C231">
+        <v>1</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C235">
+        <v>1</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C241">
+        <v>1</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243">
+        <v>3</v>
+      </c>
+      <c r="D243">
+        <v>0</v>
+      </c>
+      <c r="E243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C244">
+        <v>3</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22438,10 +25593,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDC0D5B-6DEC-481F-93A5-E40ED9D77DD6}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="E215" sqref="D215:E218"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26084,6 +29239,533 @@
         <v>62</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215">
+        <v>39</v>
+      </c>
+      <c r="D215">
+        <v>0</v>
+      </c>
+      <c r="E215">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C216">
+        <v>30</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C217">
+        <v>15</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C218">
+        <v>19</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C219">
+        <v>41</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C220">
+        <v>34</v>
+      </c>
+      <c r="D220">
+        <v>0</v>
+      </c>
+      <c r="E220">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C221">
+        <v>15</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C222">
+        <v>23</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C223">
+        <v>13</v>
+      </c>
+      <c r="D223">
+        <v>0</v>
+      </c>
+      <c r="E223">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C224">
+        <v>3</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C225">
+        <v>20</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C226">
+        <v>19</v>
+      </c>
+      <c r="D226">
+        <v>0</v>
+      </c>
+      <c r="E226">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C227">
+        <v>11</v>
+      </c>
+      <c r="D227">
+        <v>0</v>
+      </c>
+      <c r="E227">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C228">
+        <v>19</v>
+      </c>
+      <c r="D228">
+        <v>3</v>
+      </c>
+      <c r="E228">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C229">
+        <v>25</v>
+      </c>
+      <c r="D229">
+        <v>0</v>
+      </c>
+      <c r="E229">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C230">
+        <v>21</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C231">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C232">
+        <v>20</v>
+      </c>
+      <c r="D232">
+        <v>0</v>
+      </c>
+      <c r="E232">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C233">
+        <v>21</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234">
+        <v>10</v>
+      </c>
+      <c r="D234">
+        <v>0</v>
+      </c>
+      <c r="E234">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C235">
+        <v>10</v>
+      </c>
+      <c r="D235">
+        <v>0</v>
+      </c>
+      <c r="E235">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C236">
+        <v>6</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C237">
+        <v>13</v>
+      </c>
+      <c r="D237">
+        <v>0</v>
+      </c>
+      <c r="E237">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C239">
+        <v>7</v>
+      </c>
+      <c r="D239">
+        <v>2</v>
+      </c>
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C240">
+        <v>12</v>
+      </c>
+      <c r="D240">
+        <v>0</v>
+      </c>
+      <c r="E240">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C241">
+        <v>10</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C242">
+        <v>8</v>
+      </c>
+      <c r="D242">
+        <v>0</v>
+      </c>
+      <c r="E242">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C243">
+        <v>15</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="E243">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C244">
+        <v>6</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C245">
+        <v>4</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -26091,10 +29773,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4A9579-2ABE-449F-A979-F5A5DA072684}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="E217" sqref="E215:E217"/>
+    <sheetView topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="F245" sqref="F245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29737,6 +33419,533 @@
         <v>25</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C215">
+        <v>70</v>
+      </c>
+      <c r="D215">
+        <v>18</v>
+      </c>
+      <c r="E215">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C216">
+        <v>33</v>
+      </c>
+      <c r="D216">
+        <v>14</v>
+      </c>
+      <c r="E216">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C217">
+        <v>11</v>
+      </c>
+      <c r="D217">
+        <v>10</v>
+      </c>
+      <c r="E217">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C218">
+        <v>27</v>
+      </c>
+      <c r="D218">
+        <v>10</v>
+      </c>
+      <c r="E218">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C219">
+        <v>43</v>
+      </c>
+      <c r="D219">
+        <v>14</v>
+      </c>
+      <c r="E219">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C220">
+        <v>92</v>
+      </c>
+      <c r="D220">
+        <v>12</v>
+      </c>
+      <c r="E220">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C221">
+        <v>43</v>
+      </c>
+      <c r="D221">
+        <v>11</v>
+      </c>
+      <c r="E221">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222">
+        <v>46</v>
+      </c>
+      <c r="D222">
+        <v>16</v>
+      </c>
+      <c r="E222">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C223">
+        <v>14</v>
+      </c>
+      <c r="D223">
+        <v>15</v>
+      </c>
+      <c r="E223">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C224">
+        <v>21</v>
+      </c>
+      <c r="D224">
+        <v>12</v>
+      </c>
+      <c r="E224">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C225">
+        <v>36</v>
+      </c>
+      <c r="D225">
+        <v>11</v>
+      </c>
+      <c r="E225">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226">
+        <v>36</v>
+      </c>
+      <c r="D226">
+        <v>13</v>
+      </c>
+      <c r="E226">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C227">
+        <v>61</v>
+      </c>
+      <c r="D227">
+        <v>17</v>
+      </c>
+      <c r="E227">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C228">
+        <v>64</v>
+      </c>
+      <c r="D228">
+        <v>12</v>
+      </c>
+      <c r="E228">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C229">
+        <v>44</v>
+      </c>
+      <c r="D229">
+        <v>13</v>
+      </c>
+      <c r="E229">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C230">
+        <v>24</v>
+      </c>
+      <c r="D230">
+        <v>13</v>
+      </c>
+      <c r="E230">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C231">
+        <v>3</v>
+      </c>
+      <c r="D231">
+        <v>11</v>
+      </c>
+      <c r="E231">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C232">
+        <v>31</v>
+      </c>
+      <c r="D232">
+        <v>3</v>
+      </c>
+      <c r="E232">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C233">
+        <v>48</v>
+      </c>
+      <c r="D233">
+        <v>4</v>
+      </c>
+      <c r="E233">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234">
+        <v>51</v>
+      </c>
+      <c r="D234">
+        <v>6</v>
+      </c>
+      <c r="E234">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C235">
+        <v>38</v>
+      </c>
+      <c r="D235">
+        <v>3</v>
+      </c>
+      <c r="E235">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236">
+        <v>22</v>
+      </c>
+      <c r="D236">
+        <v>3</v>
+      </c>
+      <c r="E236">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C237">
+        <v>14</v>
+      </c>
+      <c r="D237">
+        <v>4</v>
+      </c>
+      <c r="E237">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238">
+        <v>24</v>
+      </c>
+      <c r="D238">
+        <v>4</v>
+      </c>
+      <c r="E238">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C239">
+        <v>8</v>
+      </c>
+      <c r="D239">
+        <v>3</v>
+      </c>
+      <c r="E239">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C240">
+        <v>23</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+      <c r="E240">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C241">
+        <v>46</v>
+      </c>
+      <c r="D241">
+        <v>1</v>
+      </c>
+      <c r="E241">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C242">
+        <v>40</v>
+      </c>
+      <c r="D242">
+        <v>2</v>
+      </c>
+      <c r="E242">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C243">
+        <v>50</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="E243">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C244">
+        <v>12</v>
+      </c>
+      <c r="D244">
+        <v>0</v>
+      </c>
+      <c r="E244">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C245">
+        <v>6</v>
+      </c>
+      <c r="D245">
+        <v>0</v>
+      </c>
+      <c r="E245">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29744,10 +33953,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A96C0A-A18D-4A9E-A2AB-42B6B5416AE0}">
-  <dimension ref="A1:E214"/>
+  <dimension ref="A1:E245"/>
   <sheetViews>
-    <sheetView topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="E215" sqref="D215:E217"/>
+    <sheetView topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33393,6 +37602,533 @@
         <v>71</v>
       </c>
     </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="14">
+        <v>44113</v>
+      </c>
+      <c r="B215" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215">
+        <v>27</v>
+      </c>
+      <c r="D215">
+        <v>3</v>
+      </c>
+      <c r="E215">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="14">
+        <v>44114</v>
+      </c>
+      <c r="B216" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216">
+        <v>94</v>
+      </c>
+      <c r="D216">
+        <v>2</v>
+      </c>
+      <c r="E216">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="14">
+        <v>44115</v>
+      </c>
+      <c r="B217" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217">
+        <v>50</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="14">
+        <v>44116</v>
+      </c>
+      <c r="B218" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C218">
+        <v>32</v>
+      </c>
+      <c r="D218">
+        <v>1</v>
+      </c>
+      <c r="E218">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="14">
+        <v>44117</v>
+      </c>
+      <c r="B219" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219">
+        <v>58</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="14">
+        <v>44118</v>
+      </c>
+      <c r="B220" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220">
+        <v>49</v>
+      </c>
+      <c r="D220">
+        <v>6</v>
+      </c>
+      <c r="E220">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="14">
+        <v>44119</v>
+      </c>
+      <c r="B221" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C221">
+        <v>45</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="14">
+        <v>44120</v>
+      </c>
+      <c r="B222" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C222">
+        <v>76</v>
+      </c>
+      <c r="D222">
+        <v>2</v>
+      </c>
+      <c r="E222">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="14">
+        <v>44121</v>
+      </c>
+      <c r="B223" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C223">
+        <v>50</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+      <c r="E223">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="14">
+        <v>44122</v>
+      </c>
+      <c r="B224" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+      <c r="D224">
+        <v>0</v>
+      </c>
+      <c r="E224">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="14">
+        <v>44123</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C225">
+        <v>24</v>
+      </c>
+      <c r="D225">
+        <v>2</v>
+      </c>
+      <c r="E225">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="14">
+        <v>44124</v>
+      </c>
+      <c r="B226" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C226">
+        <v>35</v>
+      </c>
+      <c r="D226">
+        <v>1</v>
+      </c>
+      <c r="E226">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="14">
+        <v>44125</v>
+      </c>
+      <c r="B227" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C227">
+        <v>39</v>
+      </c>
+      <c r="D227">
+        <v>4</v>
+      </c>
+      <c r="E227">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="14">
+        <v>44126</v>
+      </c>
+      <c r="B228" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C228">
+        <v>73</v>
+      </c>
+      <c r="D228">
+        <v>2</v>
+      </c>
+      <c r="E228">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="14">
+        <v>44127</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C229">
+        <v>37</v>
+      </c>
+      <c r="D229">
+        <v>2</v>
+      </c>
+      <c r="E229">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="14">
+        <v>44128</v>
+      </c>
+      <c r="B230" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C230">
+        <v>50</v>
+      </c>
+      <c r="D230">
+        <v>0</v>
+      </c>
+      <c r="E230">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="14">
+        <v>44129</v>
+      </c>
+      <c r="B231" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C231">
+        <v>19</v>
+      </c>
+      <c r="D231">
+        <v>3</v>
+      </c>
+      <c r="E231">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="14">
+        <v>44130</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C232">
+        <v>18</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="14">
+        <v>44131</v>
+      </c>
+      <c r="B233" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C233">
+        <v>49</v>
+      </c>
+      <c r="D233">
+        <v>0</v>
+      </c>
+      <c r="E233">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="14">
+        <v>44132</v>
+      </c>
+      <c r="B234" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C234">
+        <v>51</v>
+      </c>
+      <c r="D234">
+        <v>4</v>
+      </c>
+      <c r="E234">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="14">
+        <v>44133</v>
+      </c>
+      <c r="B235" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C235">
+        <v>38</v>
+      </c>
+      <c r="D235">
+        <v>3</v>
+      </c>
+      <c r="E235">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="14">
+        <v>44134</v>
+      </c>
+      <c r="B236" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C236">
+        <v>37</v>
+      </c>
+      <c r="D236">
+        <v>0</v>
+      </c>
+      <c r="E236">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="14">
+        <v>44135</v>
+      </c>
+      <c r="B237" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C237">
+        <v>60</v>
+      </c>
+      <c r="D237">
+        <v>1</v>
+      </c>
+      <c r="E237">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="14">
+        <v>44136</v>
+      </c>
+      <c r="B238" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C238">
+        <v>13</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="14">
+        <v>44137</v>
+      </c>
+      <c r="B239" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+      <c r="E239">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="14">
+        <v>44138</v>
+      </c>
+      <c r="B240" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C240">
+        <v>16</v>
+      </c>
+      <c r="D240">
+        <v>1</v>
+      </c>
+      <c r="E240">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="14">
+        <v>44139</v>
+      </c>
+      <c r="B241" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C241">
+        <v>25</v>
+      </c>
+      <c r="D241">
+        <v>0</v>
+      </c>
+      <c r="E241">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="14">
+        <v>44140</v>
+      </c>
+      <c r="B242" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C242">
+        <v>26</v>
+      </c>
+      <c r="D242">
+        <v>1</v>
+      </c>
+      <c r="E242">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="14">
+        <v>44141</v>
+      </c>
+      <c r="B243" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C243">
+        <v>27</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="E243">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="14">
+        <v>44142</v>
+      </c>
+      <c r="B244" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C244">
+        <v>36</v>
+      </c>
+      <c r="D244">
+        <v>5</v>
+      </c>
+      <c r="E244">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="14">
+        <v>44143</v>
+      </c>
+      <c r="B245" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C245">
+        <v>0</v>
+      </c>
+      <c r="D245">
+        <v>1</v>
+      </c>
+      <c r="E245">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>